<commit_message>
Change mozzarella template --no-tests
</commit_message>
<xml_diff>
--- a/app/data/static/templates/constructor_mozzarella.xlsx
+++ b/app/data/static/templates/constructor_mozzarella.xlsx
@@ -4344,7 +4344,7 @@
         <v>0</v>
       </c>
       <c r="Q66">
-        <f t="shared" ref="Q66:Q97" ca="1" si="23">IF(O66 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(P66)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(P66)))), 0)</f>
+        <f t="shared" ref="Q66:Q73" ca="1" si="23">IF(O66 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(P66)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(P66)))), 0)</f>
         <v>0</v>
       </c>
       <c r="R66">
@@ -5968,11 +5968,11 @@
       </c>
       <c r="M98" s="19"/>
       <c r="N98" s="18" t="str">
-        <f t="shared" ref="N98:N129" ca="1" si="32">IF(M98="", IF(X98=0, "", X98), IF(V98 = "", "", IF(V98/U98 = 0, "", V98/U98)))</f>
+        <f t="shared" ref="N98:N122" ca="1" si="32">IF(M98="", IF(X98=0, "", X98), IF(V98 = "", "", IF(V98/U98 = 0, "", V98/U98)))</f>
         <v/>
       </c>
       <c r="P98">
-        <f t="shared" ref="P98:P129" si="33">IF(O98 = "-", -W98,I98)</f>
+        <f t="shared" ref="P98:P122" si="33">IF(O98 = "-", -W98,I98)</f>
         <v>0</v>
       </c>
       <c r="Q98">
@@ -6000,7 +6000,7 @@
         <v>0</v>
       </c>
       <c r="W98">
-        <f t="shared" ref="W98:W129" ca="1" si="38">IF(V98 = "", "", V98/U98)</f>
+        <f t="shared" ref="W98:W122" ca="1" si="38">IF(V98 = "", "", V98/U98)</f>
         <v>0</v>
       </c>
       <c r="X98" t="str">
@@ -7880,7 +7880,7 @@
           </x14:formula2>
           <xm:sqref>L1:L122</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>'Вода SKU'!$A$1:$A$150</xm:f>
           </x14:formula1>
@@ -11281,7 +11281,7 @@
         <v>0</v>
       </c>
       <c r="Q66">
-        <f t="shared" ref="Q66:Q97" ca="1" si="23">IF(O66 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(P66)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(P66)))), 0)</f>
+        <f t="shared" ref="Q66:Q73" ca="1" si="23">IF(O66 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(P66)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(P66)))), 0)</f>
         <v>0</v>
       </c>
       <c r="R66">
@@ -12905,11 +12905,11 @@
       </c>
       <c r="M98" s="19"/>
       <c r="N98" s="18" t="str">
-        <f t="shared" ref="N98:N129" ca="1" si="32">IF(M98="", IF(X98=0, "", X98), IF(V98 = "", "", IF(V98/U98 = 0, "", V98/U98)))</f>
+        <f t="shared" ref="N98:N122" ca="1" si="32">IF(M98="", IF(X98=0, "", X98), IF(V98 = "", "", IF(V98/U98 = 0, "", V98/U98)))</f>
         <v/>
       </c>
       <c r="P98">
-        <f t="shared" ref="P98:P129" si="33">IF(O98 = "-", -W98,I98)</f>
+        <f t="shared" ref="P98:P122" si="33">IF(O98 = "-", -W98,I98)</f>
         <v>0</v>
       </c>
       <c r="Q98">
@@ -12937,7 +12937,7 @@
         <v>0</v>
       </c>
       <c r="W98">
-        <f t="shared" ref="W98:W129" ca="1" si="38">IF(V98 = "", "", V98/U98)</f>
+        <f t="shared" ref="W98:W122" ca="1" si="38">IF(V98 = "", "", V98/U98)</f>
         <v>0</v>
       </c>
       <c r="X98" t="str">
@@ -15216,9 +15216,9 @@
           </x14:formula2>
           <xm:sqref>L1:L122</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
-            <xm:f>'Соль SKU'!$A$1:$A$200</xm:f>
+            <xm:f>'Соль SKU'!$A$1:$A$150</xm:f>
           </x14:formula1>
           <xm:sqref>H2:H200</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
Fix: mozzarella line form --no-tests
</commit_message>
<xml_diff>
--- a/app/data/static/templates/constructor_mozzarella.xlsx
+++ b/app/data/static/templates/constructor_mozzarella.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="файл остатки" sheetId="1" state="visible" r:id="rId2"/>
@@ -375,14 +375,14 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -397,85 +397,6 @@
         <family val="0"/>
         <color rgb="FF000000"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF7A19A"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="false" diagonalDown="false">
-        <left style="hair"/>
-        <right style="hair"/>
-        <top style="hair"/>
-        <bottom style="hair"/>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFED1C24"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0EFD4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0EFD4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF65C295"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEBF1DE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -614,7 +535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -624,14 +545,11 @@
       <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.09"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -640,7 +558,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -650,15 +568,14 @@
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.54"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -667,7 +584,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -677,15 +594,14 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="69.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.54"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -694,7 +610,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -706,22 +622,18 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="62.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="10.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="9.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="14" style="0" width="9.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="23" min="18" style="0" width="9.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="9.09"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.09"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="9.09"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="23" min="18" style="0" width="9.09"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -777,7 +689,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -786,23 +698,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:X220"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="16" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.36"/>
@@ -822,8 +733,7 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="21" min="21" style="0" width="4.54"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="22" style="0" width="6.73"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="23" min="23" style="0" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="24" min="24" style="0" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="24" min="24" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -897,7 +807,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="16"/>
       <c r="J2" s="9" t="str">
         <f aca="true">IF(M2="", IF(O2="","",X2+(INDIRECT("S" &amp; ROW() - 1) - S2)),IF(O2="", "", INDIRECT("S" &amp; ROW() - 1) - S2))</f>
@@ -933,7 +843,7 @@
         <v/>
       </c>
       <c r="U2" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V2" s="0" t="n">
@@ -949,7 +859,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J3" s="9" t="str">
         <f aca="true">IF(M3="", IF(O3="","",X3+(INDIRECT("S" &amp; ROW() - 1) - S3)),IF(O3="", "", INDIRECT("S" &amp; ROW() - 1) - S3))</f>
         <v/>
@@ -984,7 +894,7 @@
         <v/>
       </c>
       <c r="U3" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V3" s="0" t="n">
@@ -1000,7 +910,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J4" s="9" t="str">
         <f aca="true">IF(M4="", IF(O4="","",X4+(INDIRECT("S" &amp; ROW() - 1) - S4)),IF(O4="", "", INDIRECT("S" &amp; ROW() - 1) - S4))</f>
         <v/>
@@ -1035,7 +945,7 @@
         <v/>
       </c>
       <c r="U4" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V4" s="0" t="n">
@@ -1051,7 +961,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J5" s="9" t="str">
         <f aca="true">IF(M5="", IF(O5="","",X5+(INDIRECT("S" &amp; ROW() - 1) - S5)),IF(O5="", "", INDIRECT("S" &amp; ROW() - 1) - S5))</f>
         <v/>
@@ -1086,7 +996,7 @@
         <v/>
       </c>
       <c r="U5" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V5" s="0" t="n">
@@ -1102,7 +1012,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J6" s="9" t="str">
         <f aca="true">IF(M6="", IF(O6="","",X6+(INDIRECT("S" &amp; ROW() - 1) - S6)),IF(O6="", "", INDIRECT("S" &amp; ROW() - 1) - S6))</f>
         <v/>
@@ -1137,7 +1047,7 @@
         <v/>
       </c>
       <c r="U6" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V6" s="0" t="n">
@@ -1153,7 +1063,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J7" s="9" t="str">
         <f aca="true">IF(M7="", IF(O7="","",X7+(INDIRECT("S" &amp; ROW() - 1) - S7)),IF(O7="", "", INDIRECT("S" &amp; ROW() - 1) - S7))</f>
         <v/>
@@ -1188,7 +1098,7 @@
         <v/>
       </c>
       <c r="U7" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V7" s="0" t="n">
@@ -1204,7 +1114,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J8" s="9" t="str">
         <f aca="true">IF(M8="", IF(O8="","",X8+(INDIRECT("S" &amp; ROW() - 1) - S8)),IF(O8="", "", INDIRECT("S" &amp; ROW() - 1) - S8))</f>
         <v/>
@@ -1239,7 +1149,7 @@
         <v/>
       </c>
       <c r="U8" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V8" s="0" t="n">
@@ -1255,7 +1165,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J9" s="9" t="str">
         <f aca="true">IF(M9="", IF(O9="","",X9+(INDIRECT("S" &amp; ROW() - 1) - S9)),IF(O9="", "", INDIRECT("S" &amp; ROW() - 1) - S9))</f>
         <v/>
@@ -1290,7 +1200,7 @@
         <v/>
       </c>
       <c r="U9" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V9" s="0" t="n">
@@ -1306,7 +1216,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J10" s="9" t="str">
         <f aca="true">IF(M10="", IF(O10="","",X10+(INDIRECT("S" &amp; ROW() - 1) - S10)),IF(O10="", "", INDIRECT("S" &amp; ROW() - 1) - S10))</f>
         <v/>
@@ -1341,7 +1251,7 @@
         <v/>
       </c>
       <c r="U10" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V10" s="0" t="n">
@@ -1357,7 +1267,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J11" s="9" t="str">
         <f aca="true">IF(M11="", IF(O11="","",X11+(INDIRECT("S" &amp; ROW() - 1) - S11)),IF(O11="", "", INDIRECT("S" &amp; ROW() - 1) - S11))</f>
         <v/>
@@ -1392,7 +1302,7 @@
         <v/>
       </c>
       <c r="U11" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V11" s="0" t="n">
@@ -1408,7 +1318,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J12" s="9" t="str">
         <f aca="true">IF(M12="", IF(O12="","",X12+(INDIRECT("S" &amp; ROW() - 1) - S12)),IF(O12="", "", INDIRECT("S" &amp; ROW() - 1) - S12))</f>
         <v/>
@@ -1443,7 +1353,7 @@
         <v/>
       </c>
       <c r="U12" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V12" s="0" t="n">
@@ -1459,7 +1369,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J13" s="9" t="str">
         <f aca="true">IF(M13="", IF(O13="","",X13+(INDIRECT("S" &amp; ROW() - 1) - S13)),IF(O13="", "", INDIRECT("S" &amp; ROW() - 1) - S13))</f>
         <v/>
@@ -1494,7 +1404,7 @@
         <v/>
       </c>
       <c r="U13" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V13" s="0" t="n">
@@ -1510,7 +1420,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J14" s="9" t="str">
         <f aca="true">IF(M14="", IF(O14="","",X14+(INDIRECT("S" &amp; ROW() - 1) - S14)),IF(O14="", "", INDIRECT("S" &amp; ROW() - 1) - S14))</f>
         <v/>
@@ -1545,7 +1455,7 @@
         <v/>
       </c>
       <c r="U14" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V14" s="0" t="n">
@@ -1561,7 +1471,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J15" s="9" t="str">
         <f aca="true">IF(M15="", IF(O15="","",X15+(INDIRECT("S" &amp; ROW() - 1) - S15)),IF(O15="", "", INDIRECT("S" &amp; ROW() - 1) - S15))</f>
         <v/>
@@ -1596,7 +1506,7 @@
         <v/>
       </c>
       <c r="U15" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V15" s="0" t="n">
@@ -1612,7 +1522,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J16" s="9" t="str">
         <f aca="true">IF(M16="", IF(O16="","",X16+(INDIRECT("S" &amp; ROW() - 1) - S16)),IF(O16="", "", INDIRECT("S" &amp; ROW() - 1) - S16))</f>
         <v/>
@@ -1647,7 +1557,7 @@
         <v/>
       </c>
       <c r="U16" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V16" s="0" t="n">
@@ -1663,7 +1573,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J17" s="9" t="str">
         <f aca="true">IF(M17="", IF(O17="","",X17+(INDIRECT("S" &amp; ROW() - 1) - S17)),IF(O17="", "", INDIRECT("S" &amp; ROW() - 1) - S17))</f>
         <v/>
@@ -1698,7 +1608,7 @@
         <v/>
       </c>
       <c r="U17" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V17" s="0" t="n">
@@ -1714,7 +1624,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J18" s="9" t="str">
         <f aca="true">IF(M18="", IF(O18="","",X18+(INDIRECT("S" &amp; ROW() - 1) - S18)),IF(O18="", "", INDIRECT("S" &amp; ROW() - 1) - S18))</f>
         <v/>
@@ -1749,7 +1659,7 @@
         <v/>
       </c>
       <c r="U18" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V18" s="0" t="n">
@@ -1765,7 +1675,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J19" s="9" t="str">
         <f aca="true">IF(M19="", IF(O19="","",X19+(INDIRECT("S" &amp; ROW() - 1) - S19)),IF(O19="", "", INDIRECT("S" &amp; ROW() - 1) - S19))</f>
         <v/>
@@ -1800,7 +1710,7 @@
         <v/>
       </c>
       <c r="U19" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V19" s="0" t="n">
@@ -1816,7 +1726,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J20" s="9" t="str">
         <f aca="true">IF(M20="", IF(O20="","",X20+(INDIRECT("S" &amp; ROW() - 1) - S20)),IF(O20="", "", INDIRECT("S" &amp; ROW() - 1) - S20))</f>
         <v/>
@@ -1851,7 +1761,7 @@
         <v/>
       </c>
       <c r="U20" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V20" s="0" t="n">
@@ -1867,7 +1777,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J21" s="9" t="str">
         <f aca="true">IF(M21="", IF(O21="","",X21+(INDIRECT("S" &amp; ROW() - 1) - S21)),IF(O21="", "", INDIRECT("S" &amp; ROW() - 1) - S21))</f>
         <v/>
@@ -1902,7 +1812,7 @@
         <v/>
       </c>
       <c r="U21" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V21" s="0" t="n">
@@ -1918,7 +1828,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J22" s="9" t="str">
         <f aca="true">IF(M22="", IF(O22="","",X22+(INDIRECT("S" &amp; ROW() - 1) - S22)),IF(O22="", "", INDIRECT("S" &amp; ROW() - 1) - S22))</f>
         <v/>
@@ -1953,7 +1863,7 @@
         <v/>
       </c>
       <c r="U22" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V22" s="0" t="n">
@@ -1969,7 +1879,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J23" s="9" t="str">
         <f aca="true">IF(M23="", IF(O23="","",X23+(INDIRECT("S" &amp; ROW() - 1) - S23)),IF(O23="", "", INDIRECT("S" &amp; ROW() - 1) - S23))</f>
         <v/>
@@ -2004,7 +1914,7 @@
         <v/>
       </c>
       <c r="U23" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V23" s="0" t="n">
@@ -2020,7 +1930,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J24" s="9" t="str">
         <f aca="true">IF(M24="", IF(O24="","",X24+(INDIRECT("S" &amp; ROW() - 1) - S24)),IF(O24="", "", INDIRECT("S" &amp; ROW() - 1) - S24))</f>
         <v/>
@@ -2055,7 +1965,7 @@
         <v/>
       </c>
       <c r="U24" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V24" s="0" t="n">
@@ -2071,7 +1981,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J25" s="9" t="str">
         <f aca="true">IF(M25="", IF(O25="","",X25+(INDIRECT("S" &amp; ROW() - 1) - S25)),IF(O25="", "", INDIRECT("S" &amp; ROW() - 1) - S25))</f>
         <v/>
@@ -2106,7 +2016,7 @@
         <v/>
       </c>
       <c r="U25" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V25" s="0" t="n">
@@ -2122,7 +2032,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J26" s="9" t="str">
         <f aca="true">IF(M26="", IF(O26="","",X26+(INDIRECT("S" &amp; ROW() - 1) - S26)),IF(O26="", "", INDIRECT("S" &amp; ROW() - 1) - S26))</f>
         <v/>
@@ -2157,7 +2067,7 @@
         <v/>
       </c>
       <c r="U26" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V26" s="0" t="n">
@@ -2173,7 +2083,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J27" s="9" t="str">
         <f aca="true">IF(M27="", IF(O27="","",X27+(INDIRECT("S" &amp; ROW() - 1) - S27)),IF(O27="", "", INDIRECT("S" &amp; ROW() - 1) - S27))</f>
         <v/>
@@ -2208,7 +2118,7 @@
         <v/>
       </c>
       <c r="U27" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V27" s="0" t="n">
@@ -2224,7 +2134,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J28" s="9" t="str">
         <f aca="true">IF(M28="", IF(O28="","",X28+(INDIRECT("S" &amp; ROW() - 1) - S28)),IF(O28="", "", INDIRECT("S" &amp; ROW() - 1) - S28))</f>
         <v/>
@@ -2259,7 +2169,7 @@
         <v/>
       </c>
       <c r="U28" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V28" s="0" t="n">
@@ -2275,7 +2185,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J29" s="9" t="str">
         <f aca="true">IF(M29="", IF(O29="","",X29+(INDIRECT("S" &amp; ROW() - 1) - S29)),IF(O29="", "", INDIRECT("S" &amp; ROW() - 1) - S29))</f>
         <v/>
@@ -2310,7 +2220,7 @@
         <v/>
       </c>
       <c r="U29" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V29" s="0" t="n">
@@ -2326,7 +2236,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J30" s="9" t="str">
         <f aca="true">IF(M30="", IF(O30="","",X30+(INDIRECT("S" &amp; ROW() - 1) - S30)),IF(O30="", "", INDIRECT("S" &amp; ROW() - 1) - S30))</f>
         <v/>
@@ -2361,7 +2271,7 @@
         <v/>
       </c>
       <c r="U30" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V30" s="0" t="n">
@@ -2377,7 +2287,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J31" s="9" t="str">
         <f aca="true">IF(M31="", IF(O31="","",X31+(INDIRECT("S" &amp; ROW() - 1) - S31)),IF(O31="", "", INDIRECT("S" &amp; ROW() - 1) - S31))</f>
         <v/>
@@ -2412,7 +2322,7 @@
         <v/>
       </c>
       <c r="U31" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V31" s="0" t="n">
@@ -2428,7 +2338,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J32" s="9" t="str">
         <f aca="true">IF(M32="", IF(O32="","",X32+(INDIRECT("S" &amp; ROW() - 1) - S32)),IF(O32="", "", INDIRECT("S" &amp; ROW() - 1) - S32))</f>
         <v/>
@@ -2463,7 +2373,7 @@
         <v/>
       </c>
       <c r="U32" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V32" s="0" t="n">
@@ -2479,7 +2389,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J33" s="9" t="str">
         <f aca="true">IF(M33="", IF(O33="","",X33+(INDIRECT("S" &amp; ROW() - 1) - S33)),IF(O33="", "", INDIRECT("S" &amp; ROW() - 1) - S33))</f>
         <v/>
@@ -2514,7 +2424,7 @@
         <v/>
       </c>
       <c r="U33" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V33" s="0" t="n">
@@ -2530,7 +2440,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J34" s="9" t="str">
         <f aca="true">IF(M34="", IF(O34="","",X34+(INDIRECT("S" &amp; ROW() - 1) - S34)),IF(O34="", "", INDIRECT("S" &amp; ROW() - 1) - S34))</f>
         <v/>
@@ -2565,7 +2475,7 @@
         <v/>
       </c>
       <c r="U34" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V34" s="0" t="n">
@@ -2581,7 +2491,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J35" s="9" t="str">
         <f aca="true">IF(M35="", IF(O35="","",X35+(INDIRECT("S" &amp; ROW() - 1) - S35)),IF(O35="", "", INDIRECT("S" &amp; ROW() - 1) - S35))</f>
         <v/>
@@ -2616,7 +2526,7 @@
         <v/>
       </c>
       <c r="U35" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V35" s="0" t="n">
@@ -2632,7 +2542,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J36" s="9" t="str">
         <f aca="true">IF(M36="", IF(O36="","",X36+(INDIRECT("S" &amp; ROW() - 1) - S36)),IF(O36="", "", INDIRECT("S" &amp; ROW() - 1) - S36))</f>
         <v/>
@@ -2667,7 +2577,7 @@
         <v/>
       </c>
       <c r="U36" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V36" s="0" t="n">
@@ -2683,7 +2593,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J37" s="9" t="str">
         <f aca="true">IF(M37="", IF(O37="","",X37+(INDIRECT("S" &amp; ROW() - 1) - S37)),IF(O37="", "", INDIRECT("S" &amp; ROW() - 1) - S37))</f>
         <v/>
@@ -2718,7 +2628,7 @@
         <v/>
       </c>
       <c r="U37" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V37" s="0" t="n">
@@ -2734,7 +2644,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J38" s="9" t="str">
         <f aca="true">IF(M38="", IF(O38="","",X38+(INDIRECT("S" &amp; ROW() - 1) - S38)),IF(O38="", "", INDIRECT("S" &amp; ROW() - 1) - S38))</f>
         <v/>
@@ -2769,7 +2679,7 @@
         <v/>
       </c>
       <c r="U38" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V38" s="0" t="n">
@@ -2785,7 +2695,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J39" s="9" t="str">
         <f aca="true">IF(M39="", IF(O39="","",X39+(INDIRECT("S" &amp; ROW() - 1) - S39)),IF(O39="", "", INDIRECT("S" &amp; ROW() - 1) - S39))</f>
         <v/>
@@ -2820,7 +2730,7 @@
         <v/>
       </c>
       <c r="U39" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V39" s="0" t="n">
@@ -2836,7 +2746,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J40" s="9" t="str">
         <f aca="true">IF(M40="", IF(O40="","",X40+(INDIRECT("S" &amp; ROW() - 1) - S40)),IF(O40="", "", INDIRECT("S" &amp; ROW() - 1) - S40))</f>
         <v/>
@@ -2871,7 +2781,7 @@
         <v/>
       </c>
       <c r="U40" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V40" s="0" t="n">
@@ -2887,7 +2797,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J41" s="9" t="str">
         <f aca="true">IF(M41="", IF(O41="","",X41+(INDIRECT("S" &amp; ROW() - 1) - S41)),IF(O41="", "", INDIRECT("S" &amp; ROW() - 1) - S41))</f>
         <v/>
@@ -2922,7 +2832,7 @@
         <v/>
       </c>
       <c r="U41" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V41" s="0" t="n">
@@ -2938,7 +2848,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J42" s="9" t="str">
         <f aca="true">IF(M42="", IF(O42="","",X42+(INDIRECT("S" &amp; ROW() - 1) - S42)),IF(O42="", "", INDIRECT("S" &amp; ROW() - 1) - S42))</f>
         <v/>
@@ -2973,7 +2883,7 @@
         <v/>
       </c>
       <c r="U42" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V42" s="0" t="n">
@@ -2989,7 +2899,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J43" s="9" t="str">
         <f aca="true">IF(M43="", IF(O43="","",X43+(INDIRECT("S" &amp; ROW() - 1) - S43)),IF(O43="", "", INDIRECT("S" &amp; ROW() - 1) - S43))</f>
         <v/>
@@ -3024,7 +2934,7 @@
         <v/>
       </c>
       <c r="U43" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V43" s="0" t="n">
@@ -3040,7 +2950,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J44" s="9" t="str">
         <f aca="true">IF(M44="", IF(O44="","",X44+(INDIRECT("S" &amp; ROW() - 1) - S44)),IF(O44="", "", INDIRECT("S" &amp; ROW() - 1) - S44))</f>
         <v/>
@@ -3075,7 +2985,7 @@
         <v/>
       </c>
       <c r="U44" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V44" s="0" t="n">
@@ -3091,7 +3001,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J45" s="9" t="str">
         <f aca="true">IF(M45="", IF(O45="","",X45+(INDIRECT("S" &amp; ROW() - 1) - S45)),IF(O45="", "", INDIRECT("S" &amp; ROW() - 1) - S45))</f>
         <v/>
@@ -3126,7 +3036,7 @@
         <v/>
       </c>
       <c r="U45" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V45" s="0" t="n">
@@ -3142,7 +3052,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J46" s="9" t="str">
         <f aca="true">IF(M46="", IF(O46="","",X46+(INDIRECT("S" &amp; ROW() - 1) - S46)),IF(O46="", "", INDIRECT("S" &amp; ROW() - 1) - S46))</f>
         <v/>
@@ -3177,7 +3087,7 @@
         <v/>
       </c>
       <c r="U46" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V46" s="0" t="n">
@@ -3193,7 +3103,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J47" s="9" t="str">
         <f aca="true">IF(M47="", IF(O47="","",X47+(INDIRECT("S" &amp; ROW() - 1) - S47)),IF(O47="", "", INDIRECT("S" &amp; ROW() - 1) - S47))</f>
         <v/>
@@ -3228,7 +3138,7 @@
         <v/>
       </c>
       <c r="U47" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V47" s="0" t="n">
@@ -3244,7 +3154,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J48" s="9" t="str">
         <f aca="true">IF(M48="", IF(O48="","",X48+(INDIRECT("S" &amp; ROW() - 1) - S48)),IF(O48="", "", INDIRECT("S" &amp; ROW() - 1) - S48))</f>
         <v/>
@@ -3279,7 +3189,7 @@
         <v/>
       </c>
       <c r="U48" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V48" s="0" t="n">
@@ -3295,7 +3205,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J49" s="9" t="str">
         <f aca="true">IF(M49="", IF(O49="","",X49+(INDIRECT("S" &amp; ROW() - 1) - S49)),IF(O49="", "", INDIRECT("S" &amp; ROW() - 1) - S49))</f>
         <v/>
@@ -3330,7 +3240,7 @@
         <v/>
       </c>
       <c r="U49" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V49" s="0" t="n">
@@ -3346,7 +3256,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J50" s="9" t="str">
         <f aca="true">IF(M50="", IF(O50="","",X50+(INDIRECT("S" &amp; ROW() - 1) - S50)),IF(O50="", "", INDIRECT("S" &amp; ROW() - 1) - S50))</f>
         <v/>
@@ -3381,7 +3291,7 @@
         <v/>
       </c>
       <c r="U50" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V50" s="0" t="n">
@@ -3397,7 +3307,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J51" s="9" t="str">
         <f aca="true">IF(M51="", IF(O51="","",X51+(INDIRECT("S" &amp; ROW() - 1) - S51)),IF(O51="", "", INDIRECT("S" &amp; ROW() - 1) - S51))</f>
         <v/>
@@ -3432,7 +3342,7 @@
         <v/>
       </c>
       <c r="U51" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V51" s="0" t="n">
@@ -3448,7 +3358,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J52" s="9" t="str">
         <f aca="true">IF(M52="", IF(O52="","",X52+(INDIRECT("S" &amp; ROW() - 1) - S52)),IF(O52="", "", INDIRECT("S" &amp; ROW() - 1) - S52))</f>
         <v/>
@@ -3483,7 +3393,7 @@
         <v/>
       </c>
       <c r="U52" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V52" s="0" t="n">
@@ -3499,7 +3409,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J53" s="9" t="str">
         <f aca="true">IF(M53="", IF(O53="","",X53+(INDIRECT("S" &amp; ROW() - 1) - S53)),IF(O53="", "", INDIRECT("S" &amp; ROW() - 1) - S53))</f>
         <v/>
@@ -3534,7 +3444,7 @@
         <v/>
       </c>
       <c r="U53" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V53" s="0" t="n">
@@ -3550,7 +3460,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J54" s="9" t="str">
         <f aca="true">IF(M54="", IF(O54="","",X54+(INDIRECT("S" &amp; ROW() - 1) - S54)),IF(O54="", "", INDIRECT("S" &amp; ROW() - 1) - S54))</f>
         <v/>
@@ -3585,7 +3495,7 @@
         <v/>
       </c>
       <c r="U54" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V54" s="0" t="n">
@@ -3601,7 +3511,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J55" s="9" t="str">
         <f aca="true">IF(M55="", IF(O55="","",X55+(INDIRECT("S" &amp; ROW() - 1) - S55)),IF(O55="", "", INDIRECT("S" &amp; ROW() - 1) - S55))</f>
         <v/>
@@ -3636,7 +3546,7 @@
         <v/>
       </c>
       <c r="U55" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V55" s="0" t="n">
@@ -3652,7 +3562,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J56" s="9" t="str">
         <f aca="true">IF(M56="", IF(O56="","",X56+(INDIRECT("S" &amp; ROW() - 1) - S56)),IF(O56="", "", INDIRECT("S" &amp; ROW() - 1) - S56))</f>
         <v/>
@@ -3687,7 +3597,7 @@
         <v/>
       </c>
       <c r="U56" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V56" s="0" t="n">
@@ -3703,7 +3613,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J57" s="9" t="str">
         <f aca="true">IF(M57="", IF(O57="","",X57+(INDIRECT("S" &amp; ROW() - 1) - S57)),IF(O57="", "", INDIRECT("S" &amp; ROW() - 1) - S57))</f>
         <v/>
@@ -3738,7 +3648,7 @@
         <v/>
       </c>
       <c r="U57" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V57" s="0" t="n">
@@ -3754,7 +3664,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J58" s="9" t="str">
         <f aca="true">IF(M58="", IF(O58="","",X58+(INDIRECT("S" &amp; ROW() - 1) - S58)),IF(O58="", "", INDIRECT("S" &amp; ROW() - 1) - S58))</f>
         <v/>
@@ -3789,7 +3699,7 @@
         <v/>
       </c>
       <c r="U58" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V58" s="0" t="n">
@@ -3805,7 +3715,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J59" s="9" t="str">
         <f aca="true">IF(M59="", IF(O59="","",X59+(INDIRECT("S" &amp; ROW() - 1) - S59)),IF(O59="", "", INDIRECT("S" &amp; ROW() - 1) - S59))</f>
         <v/>
@@ -3840,7 +3750,7 @@
         <v/>
       </c>
       <c r="U59" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V59" s="0" t="n">
@@ -3856,7 +3766,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J60" s="9" t="str">
         <f aca="true">IF(M60="", IF(O60="","",X60+(INDIRECT("S" &amp; ROW() - 1) - S60)),IF(O60="", "", INDIRECT("S" &amp; ROW() - 1) - S60))</f>
         <v/>
@@ -3891,7 +3801,7 @@
         <v/>
       </c>
       <c r="U60" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V60" s="0" t="n">
@@ -3907,7 +3817,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J61" s="9" t="str">
         <f aca="true">IF(M61="", IF(O61="","",X61+(INDIRECT("S" &amp; ROW() - 1) - S61)),IF(O61="", "", INDIRECT("S" &amp; ROW() - 1) - S61))</f>
         <v/>
@@ -3942,7 +3852,7 @@
         <v/>
       </c>
       <c r="U61" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V61" s="0" t="n">
@@ -3958,7 +3868,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J62" s="9" t="str">
         <f aca="true">IF(M62="", IF(O62="","",X62+(INDIRECT("S" &amp; ROW() - 1) - S62)),IF(O62="", "", INDIRECT("S" &amp; ROW() - 1) - S62))</f>
         <v/>
@@ -3993,7 +3903,7 @@
         <v/>
       </c>
       <c r="U62" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V62" s="0" t="n">
@@ -4009,7 +3919,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J63" s="9" t="str">
         <f aca="true">IF(M63="", IF(O63="","",X63+(INDIRECT("S" &amp; ROW() - 1) - S63)),IF(O63="", "", INDIRECT("S" &amp; ROW() - 1) - S63))</f>
         <v/>
@@ -4044,7 +3954,7 @@
         <v/>
       </c>
       <c r="U63" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V63" s="0" t="n">
@@ -4060,7 +3970,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J64" s="9" t="str">
         <f aca="true">IF(M64="", IF(O64="","",X64+(INDIRECT("S" &amp; ROW() - 1) - S64)),IF(O64="", "", INDIRECT("S" &amp; ROW() - 1) - S64))</f>
         <v/>
@@ -4095,7 +4005,7 @@
         <v/>
       </c>
       <c r="U64" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V64" s="0" t="n">
@@ -4111,7 +4021,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J65" s="9" t="str">
         <f aca="true">IF(M65="", IF(O65="","",X65+(INDIRECT("S" &amp; ROW() - 1) - S65)),IF(O65="", "", INDIRECT("S" &amp; ROW() - 1) - S65))</f>
         <v/>
@@ -4146,7 +4056,7 @@
         <v/>
       </c>
       <c r="U65" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V65" s="0" t="n">
@@ -4162,7 +4072,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J66" s="9" t="str">
         <f aca="true">IF(M66="", IF(O66="","",X66+(INDIRECT("S" &amp; ROW() - 1) - S66)),IF(O66="", "", INDIRECT("S" &amp; ROW() - 1) - S66))</f>
         <v/>
@@ -4197,7 +4107,7 @@
         <v/>
       </c>
       <c r="U66" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V66" s="0" t="n">
@@ -4213,7 +4123,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J67" s="9" t="str">
         <f aca="true">IF(M67="", IF(O67="","",X67+(INDIRECT("S" &amp; ROW() - 1) - S67)),IF(O67="", "", INDIRECT("S" &amp; ROW() - 1) - S67))</f>
         <v/>
@@ -4248,7 +4158,7 @@
         <v/>
       </c>
       <c r="U67" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V67" s="0" t="n">
@@ -4264,7 +4174,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J68" s="9" t="str">
         <f aca="true">IF(M68="", IF(O68="","",X68+(INDIRECT("S" &amp; ROW() - 1) - S68)),IF(O68="", "", INDIRECT("S" &amp; ROW() - 1) - S68))</f>
         <v/>
@@ -4299,7 +4209,7 @@
         <v/>
       </c>
       <c r="U68" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V68" s="0" t="n">
@@ -4315,7 +4225,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J69" s="9" t="str">
         <f aca="true">IF(M69="", IF(O69="","",X69+(INDIRECT("S" &amp; ROW() - 1) - S69)),IF(O69="", "", INDIRECT("S" &amp; ROW() - 1) - S69))</f>
         <v/>
@@ -4350,7 +4260,7 @@
         <v/>
       </c>
       <c r="U69" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V69" s="0" t="n">
@@ -4366,7 +4276,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J70" s="9" t="str">
         <f aca="true">IF(M70="", IF(O70="","",X70+(INDIRECT("S" &amp; ROW() - 1) - S70)),IF(O70="", "", INDIRECT("S" &amp; ROW() - 1) - S70))</f>
         <v/>
@@ -4401,7 +4311,7 @@
         <v/>
       </c>
       <c r="U70" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V70" s="0" t="n">
@@ -4417,7 +4327,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J71" s="9" t="str">
         <f aca="true">IF(M71="", IF(O71="","",X71+(INDIRECT("S" &amp; ROW() - 1) - S71)),IF(O71="", "", INDIRECT("S" &amp; ROW() - 1) - S71))</f>
         <v/>
@@ -4452,7 +4362,7 @@
         <v/>
       </c>
       <c r="U71" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V71" s="0" t="n">
@@ -4468,7 +4378,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J72" s="9" t="str">
         <f aca="true">IF(M72="", IF(O72="","",X72+(INDIRECT("S" &amp; ROW() - 1) - S72)),IF(O72="", "", INDIRECT("S" &amp; ROW() - 1) - S72))</f>
         <v/>
@@ -4503,7 +4413,7 @@
         <v/>
       </c>
       <c r="U72" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V72" s="0" t="n">
@@ -4519,7 +4429,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J73" s="9" t="str">
         <f aca="true">IF(M73="", IF(O73="","",X73+(INDIRECT("S" &amp; ROW() - 1) - S73)),IF(O73="", "", INDIRECT("S" &amp; ROW() - 1) - S73))</f>
         <v/>
@@ -4554,7 +4464,7 @@
         <v/>
       </c>
       <c r="U73" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V73" s="0" t="n">
@@ -4570,7 +4480,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J74" s="9" t="str">
         <f aca="true">IF(M74="", IF(O74="","",X74+(INDIRECT("S" &amp; ROW() - 1) - S74)),IF(O74="", "", INDIRECT("S" &amp; ROW() - 1) - S74))</f>
         <v/>
@@ -4605,7 +4515,7 @@
         <v/>
       </c>
       <c r="U74" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V74" s="0" t="n">
@@ -4621,7 +4531,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J75" s="9" t="str">
         <f aca="true">IF(M75="", IF(O75="","",X75+(INDIRECT("S" &amp; ROW() - 1) - S75)),IF(O75="", "", INDIRECT("S" &amp; ROW() - 1) - S75))</f>
         <v/>
@@ -4656,7 +4566,7 @@
         <v/>
       </c>
       <c r="U75" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V75" s="0" t="n">
@@ -4672,7 +4582,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J76" s="9" t="str">
         <f aca="true">IF(M76="", IF(O76="","",X76+(INDIRECT("S" &amp; ROW() - 1) - S76)),IF(O76="", "", INDIRECT("S" &amp; ROW() - 1) - S76))</f>
         <v/>
@@ -4707,7 +4617,7 @@
         <v/>
       </c>
       <c r="U76" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V76" s="0" t="n">
@@ -4723,7 +4633,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J77" s="9" t="str">
         <f aca="true">IF(M77="", IF(O77="","",X77+(INDIRECT("S" &amp; ROW() - 1) - S77)),IF(O77="", "", INDIRECT("S" &amp; ROW() - 1) - S77))</f>
         <v/>
@@ -4758,7 +4668,7 @@
         <v/>
       </c>
       <c r="U77" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V77" s="0" t="n">
@@ -4774,7 +4684,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J78" s="9" t="str">
         <f aca="true">IF(M78="", IF(O78="","",X78+(INDIRECT("S" &amp; ROW() - 1) - S78)),IF(O78="", "", INDIRECT("S" &amp; ROW() - 1) - S78))</f>
         <v/>
@@ -4809,7 +4719,7 @@
         <v/>
       </c>
       <c r="U78" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V78" s="0" t="n">
@@ -4825,7 +4735,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J79" s="9" t="str">
         <f aca="true">IF(M79="", IF(O79="","",X79+(INDIRECT("S" &amp; ROW() - 1) - S79)),IF(O79="", "", INDIRECT("S" &amp; ROW() - 1) - S79))</f>
         <v/>
@@ -4860,7 +4770,7 @@
         <v/>
       </c>
       <c r="U79" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V79" s="0" t="n">
@@ -4876,7 +4786,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J80" s="9" t="str">
         <f aca="true">IF(M80="", IF(O80="","",X80+(INDIRECT("S" &amp; ROW() - 1) - S80)),IF(O80="", "", INDIRECT("S" &amp; ROW() - 1) - S80))</f>
         <v/>
@@ -4911,7 +4821,7 @@
         <v/>
       </c>
       <c r="U80" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V80" s="0" t="n">
@@ -4927,7 +4837,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J81" s="9" t="str">
         <f aca="true">IF(M81="", IF(O81="","",X81+(INDIRECT("S" &amp; ROW() - 1) - S81)),IF(O81="", "", INDIRECT("S" &amp; ROW() - 1) - S81))</f>
         <v/>
@@ -4962,7 +4872,7 @@
         <v/>
       </c>
       <c r="U81" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V81" s="0" t="n">
@@ -4978,7 +4888,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J82" s="9" t="str">
         <f aca="true">IF(M82="", IF(O82="","",X82+(INDIRECT("S" &amp; ROW() - 1) - S82)),IF(O82="", "", INDIRECT("S" &amp; ROW() - 1) - S82))</f>
         <v/>
@@ -5013,7 +4923,7 @@
         <v/>
       </c>
       <c r="U82" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V82" s="0" t="n">
@@ -5029,7 +4939,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J83" s="9" t="str">
         <f aca="true">IF(M83="", IF(O83="","",X83+(INDIRECT("S" &amp; ROW() - 1) - S83)),IF(O83="", "", INDIRECT("S" &amp; ROW() - 1) - S83))</f>
         <v/>
@@ -5064,7 +4974,7 @@
         <v/>
       </c>
       <c r="U83" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V83" s="0" t="n">
@@ -5080,7 +4990,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J84" s="9" t="str">
         <f aca="true">IF(M84="", IF(O84="","",X84+(INDIRECT("S" &amp; ROW() - 1) - S84)),IF(O84="", "", INDIRECT("S" &amp; ROW() - 1) - S84))</f>
         <v/>
@@ -5115,7 +5025,7 @@
         <v/>
       </c>
       <c r="U84" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V84" s="0" t="n">
@@ -5131,7 +5041,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J85" s="9" t="str">
         <f aca="true">IF(M85="", IF(O85="","",X85+(INDIRECT("S" &amp; ROW() - 1) - S85)),IF(O85="", "", INDIRECT("S" &amp; ROW() - 1) - S85))</f>
         <v/>
@@ -5166,7 +5076,7 @@
         <v/>
       </c>
       <c r="U85" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V85" s="0" t="n">
@@ -5182,7 +5092,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J86" s="9" t="str">
         <f aca="true">IF(M86="", IF(O86="","",X86+(INDIRECT("S" &amp; ROW() - 1) - S86)),IF(O86="", "", INDIRECT("S" &amp; ROW() - 1) - S86))</f>
         <v/>
@@ -5217,7 +5127,7 @@
         <v/>
       </c>
       <c r="U86" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V86" s="0" t="n">
@@ -5233,7 +5143,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J87" s="9" t="str">
         <f aca="true">IF(M87="", IF(O87="","",X87+(INDIRECT("S" &amp; ROW() - 1) - S87)),IF(O87="", "", INDIRECT("S" &amp; ROW() - 1) - S87))</f>
         <v/>
@@ -5268,7 +5178,7 @@
         <v/>
       </c>
       <c r="U87" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V87" s="0" t="n">
@@ -5284,7 +5194,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J88" s="9" t="str">
         <f aca="true">IF(M88="", IF(O88="","",X88+(INDIRECT("S" &amp; ROW() - 1) - S88)),IF(O88="", "", INDIRECT("S" &amp; ROW() - 1) - S88))</f>
         <v/>
@@ -5319,7 +5229,7 @@
         <v/>
       </c>
       <c r="U88" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V88" s="0" t="n">
@@ -5335,7 +5245,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J89" s="9" t="str">
         <f aca="true">IF(M89="", IF(O89="","",X89+(INDIRECT("S" &amp; ROW() - 1) - S89)),IF(O89="", "", INDIRECT("S" &amp; ROW() - 1) - S89))</f>
         <v/>
@@ -5370,7 +5280,7 @@
         <v/>
       </c>
       <c r="U89" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V89" s="0" t="n">
@@ -5386,7 +5296,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J90" s="9" t="str">
         <f aca="true">IF(M90="", IF(O90="","",X90+(INDIRECT("S" &amp; ROW() - 1) - S90)),IF(O90="", "", INDIRECT("S" &amp; ROW() - 1) - S90))</f>
         <v/>
@@ -5421,7 +5331,7 @@
         <v/>
       </c>
       <c r="U90" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V90" s="0" t="n">
@@ -5437,7 +5347,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J91" s="9" t="str">
         <f aca="true">IF(M91="", IF(O91="","",X91+(INDIRECT("S" &amp; ROW() - 1) - S91)),IF(O91="", "", INDIRECT("S" &amp; ROW() - 1) - S91))</f>
         <v/>
@@ -5472,7 +5382,7 @@
         <v/>
       </c>
       <c r="U91" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V91" s="0" t="n">
@@ -5488,7 +5398,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J92" s="9" t="str">
         <f aca="true">IF(M92="", IF(O92="","",X92+(INDIRECT("S" &amp; ROW() - 1) - S92)),IF(O92="", "", INDIRECT("S" &amp; ROW() - 1) - S92))</f>
         <v/>
@@ -5523,7 +5433,7 @@
         <v/>
       </c>
       <c r="U92" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V92" s="0" t="n">
@@ -5539,7 +5449,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J93" s="9" t="str">
         <f aca="true">IF(M93="", IF(O93="","",X93+(INDIRECT("S" &amp; ROW() - 1) - S93)),IF(O93="", "", INDIRECT("S" &amp; ROW() - 1) - S93))</f>
         <v/>
@@ -5574,7 +5484,7 @@
         <v/>
       </c>
       <c r="U93" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V93" s="0" t="n">
@@ -5590,7 +5500,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J94" s="9" t="str">
         <f aca="true">IF(M94="", IF(O94="","",X94+(INDIRECT("S" &amp; ROW() - 1) - S94)),IF(O94="", "", INDIRECT("S" &amp; ROW() - 1) - S94))</f>
         <v/>
@@ -5625,7 +5535,7 @@
         <v/>
       </c>
       <c r="U94" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V94" s="0" t="n">
@@ -5641,7 +5551,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J95" s="9" t="str">
         <f aca="true">IF(M95="", IF(O95="","",X95+(INDIRECT("S" &amp; ROW() - 1) - S95)),IF(O95="", "", INDIRECT("S" &amp; ROW() - 1) - S95))</f>
         <v/>
@@ -5676,7 +5586,7 @@
         <v/>
       </c>
       <c r="U95" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V95" s="0" t="n">
@@ -5692,7 +5602,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J96" s="9" t="str">
         <f aca="true">IF(M96="", IF(O96="","",X96+(INDIRECT("S" &amp; ROW() - 1) - S96)),IF(O96="", "", INDIRECT("S" &amp; ROW() - 1) - S96))</f>
         <v/>
@@ -5727,7 +5637,7 @@
         <v/>
       </c>
       <c r="U96" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V96" s="0" t="n">
@@ -5743,7 +5653,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J97" s="9" t="str">
         <f aca="true">IF(M97="", IF(O97="","",X97+(INDIRECT("S" &amp; ROW() - 1) - S97)),IF(O97="", "", INDIRECT("S" &amp; ROW() - 1) - S97))</f>
         <v/>
@@ -5778,7 +5688,7 @@
         <v/>
       </c>
       <c r="U97" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V97" s="0" t="n">
@@ -5794,7 +5704,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J98" s="9" t="str">
         <f aca="true">IF(M98="", IF(O98="","",X98+(INDIRECT("S" &amp; ROW() - 1) - S98)),IF(O98="", "", INDIRECT("S" &amp; ROW() - 1) - S98))</f>
         <v/>
@@ -5829,7 +5739,7 @@
         <v/>
       </c>
       <c r="U98" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V98" s="0" t="n">
@@ -5845,7 +5755,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J99" s="9" t="str">
         <f aca="true">IF(M99="", IF(O99="","",X99+(INDIRECT("S" &amp; ROW() - 1) - S99)),IF(O99="", "", INDIRECT("S" &amp; ROW() - 1) - S99))</f>
         <v/>
@@ -5880,7 +5790,7 @@
         <v/>
       </c>
       <c r="U99" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V99" s="0" t="n">
@@ -5896,7 +5806,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J100" s="9" t="str">
         <f aca="true">IF(M100="", IF(O100="","",X100+(INDIRECT("S" &amp; ROW() - 1) - S100)),IF(O100="", "", INDIRECT("S" &amp; ROW() - 1) - S100))</f>
         <v/>
@@ -5931,7 +5841,7 @@
         <v/>
       </c>
       <c r="U100" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V100" s="0" t="n">
@@ -5947,7 +5857,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J101" s="9" t="str">
         <f aca="true">IF(M101="", IF(O101="","",X101+(INDIRECT("S" &amp; ROW() - 1) - S101)),IF(O101="", "", INDIRECT("S" &amp; ROW() - 1) - S101))</f>
         <v/>
@@ -5982,7 +5892,7 @@
         <v/>
       </c>
       <c r="U101" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V101" s="0" t="n">
@@ -5998,7 +5908,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J102" s="9" t="str">
         <f aca="true">IF(M102="", IF(O102="","",X102+(INDIRECT("S" &amp; ROW() - 1) - S102)),IF(O102="", "", INDIRECT("S" &amp; ROW() - 1) - S102))</f>
         <v/>
@@ -6033,7 +5943,7 @@
         <v/>
       </c>
       <c r="U102" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V102" s="0" t="n">
@@ -6049,7 +5959,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J103" s="9" t="str">
         <f aca="true">IF(M103="", IF(O103="","",X103+(INDIRECT("S" &amp; ROW() - 1) - S103)),IF(O103="", "", INDIRECT("S" &amp; ROW() - 1) - S103))</f>
         <v/>
@@ -6084,7 +5994,7 @@
         <v/>
       </c>
       <c r="U103" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V103" s="0" t="n">
@@ -6100,7 +6010,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J104" s="9" t="str">
         <f aca="true">IF(M104="", IF(O104="","",X104+(INDIRECT("S" &amp; ROW() - 1) - S104)),IF(O104="", "", INDIRECT("S" &amp; ROW() - 1) - S104))</f>
         <v/>
@@ -6135,7 +6045,7 @@
         <v/>
       </c>
       <c r="U104" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V104" s="0" t="n">
@@ -6151,7 +6061,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J105" s="9" t="str">
         <f aca="true">IF(M105="", IF(O105="","",X105+(INDIRECT("S" &amp; ROW() - 1) - S105)),IF(O105="", "", INDIRECT("S" &amp; ROW() - 1) - S105))</f>
         <v/>
@@ -6186,7 +6096,7 @@
         <v/>
       </c>
       <c r="U105" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V105" s="0" t="n">
@@ -6202,7 +6112,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J106" s="9" t="str">
         <f aca="true">IF(M106="", IF(O106="","",X106+(INDIRECT("S" &amp; ROW() - 1) - S106)),IF(O106="", "", INDIRECT("S" &amp; ROW() - 1) - S106))</f>
         <v/>
@@ -6237,7 +6147,7 @@
         <v/>
       </c>
       <c r="U106" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V106" s="0" t="n">
@@ -6253,7 +6163,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J107" s="9" t="str">
         <f aca="true">IF(M107="", IF(O107="","",X107+(INDIRECT("S" &amp; ROW() - 1) - S107)),IF(O107="", "", INDIRECT("S" &amp; ROW() - 1) - S107))</f>
         <v/>
@@ -6288,7 +6198,7 @@
         <v/>
       </c>
       <c r="U107" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V107" s="0" t="n">
@@ -6304,7 +6214,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J108" s="9" t="str">
         <f aca="true">IF(M108="", IF(O108="","",X108+(INDIRECT("S" &amp; ROW() - 1) - S108)),IF(O108="", "", INDIRECT("S" &amp; ROW() - 1) - S108))</f>
         <v/>
@@ -6339,7 +6249,7 @@
         <v/>
       </c>
       <c r="U108" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V108" s="0" t="n">
@@ -6355,7 +6265,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J109" s="9" t="str">
         <f aca="true">IF(M109="", IF(O109="","",X109+(INDIRECT("S" &amp; ROW() - 1) - S109)),IF(O109="", "", INDIRECT("S" &amp; ROW() - 1) - S109))</f>
         <v/>
@@ -6390,7 +6300,7 @@
         <v/>
       </c>
       <c r="U109" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V109" s="0" t="n">
@@ -6406,7 +6316,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J110" s="9" t="str">
         <f aca="true">IF(M110="", IF(O110="","",X110+(INDIRECT("S" &amp; ROW() - 1) - S110)),IF(O110="", "", INDIRECT("S" &amp; ROW() - 1) - S110))</f>
         <v/>
@@ -6441,7 +6351,7 @@
         <v/>
       </c>
       <c r="U110" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V110" s="0" t="n">
@@ -6457,7 +6367,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J111" s="9" t="str">
         <f aca="true">IF(M111="", IF(O111="","",X111+(INDIRECT("S" &amp; ROW() - 1) - S111)),IF(O111="", "", INDIRECT("S" &amp; ROW() - 1) - S111))</f>
         <v/>
@@ -6492,7 +6402,7 @@
         <v/>
       </c>
       <c r="U111" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V111" s="0" t="n">
@@ -6508,7 +6418,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J112" s="9" t="str">
         <f aca="true">IF(M112="", IF(O112="","",X112+(INDIRECT("S" &amp; ROW() - 1) - S112)),IF(O112="", "", INDIRECT("S" &amp; ROW() - 1) - S112))</f>
         <v/>
@@ -6543,7 +6453,7 @@
         <v/>
       </c>
       <c r="U112" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V112" s="0" t="n">
@@ -6559,7 +6469,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J113" s="9" t="str">
         <f aca="true">IF(M113="", IF(O113="","",X113+(INDIRECT("S" &amp; ROW() - 1) - S113)),IF(O113="", "", INDIRECT("S" &amp; ROW() - 1) - S113))</f>
         <v/>
@@ -6594,7 +6504,7 @@
         <v/>
       </c>
       <c r="U113" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V113" s="0" t="n">
@@ -6610,7 +6520,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J114" s="9" t="str">
         <f aca="true">IF(M114="", IF(O114="","",X114+(INDIRECT("S" &amp; ROW() - 1) - S114)),IF(O114="", "", INDIRECT("S" &amp; ROW() - 1) - S114))</f>
         <v/>
@@ -6645,7 +6555,7 @@
         <v/>
       </c>
       <c r="U114" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V114" s="0" t="n">
@@ -6661,7 +6571,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J115" s="9" t="str">
         <f aca="true">IF(M115="", IF(O115="","",X115+(INDIRECT("S" &amp; ROW() - 1) - S115)),IF(O115="", "", INDIRECT("S" &amp; ROW() - 1) - S115))</f>
         <v/>
@@ -6696,7 +6606,7 @@
         <v/>
       </c>
       <c r="U115" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V115" s="0" t="n">
@@ -6712,7 +6622,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J116" s="9" t="str">
         <f aca="true">IF(M116="", IF(O116="","",X116+(INDIRECT("S" &amp; ROW() - 1) - S116)),IF(O116="", "", INDIRECT("S" &amp; ROW() - 1) - S116))</f>
         <v/>
@@ -6747,7 +6657,7 @@
         <v/>
       </c>
       <c r="U116" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V116" s="0" t="n">
@@ -6763,7 +6673,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J117" s="9" t="str">
         <f aca="true">IF(M117="", IF(O117="","",X117+(INDIRECT("S" &amp; ROW() - 1) - S117)),IF(O117="", "", INDIRECT("S" &amp; ROW() - 1) - S117))</f>
         <v/>
@@ -6798,7 +6708,7 @@
         <v/>
       </c>
       <c r="U117" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V117" s="0" t="n">
@@ -6814,7 +6724,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J118" s="9" t="str">
         <f aca="true">IF(M118="", IF(O118="","",X118+(INDIRECT("S" &amp; ROW() - 1) - S118)),IF(O118="", "", INDIRECT("S" &amp; ROW() - 1) - S118))</f>
         <v/>
@@ -6849,7 +6759,7 @@
         <v/>
       </c>
       <c r="U118" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V118" s="0" t="n">
@@ -6865,7 +6775,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J119" s="9" t="str">
         <f aca="true">IF(M119="", IF(O119="","",X119+(INDIRECT("S" &amp; ROW() - 1) - S119)),IF(O119="", "", INDIRECT("S" &amp; ROW() - 1) - S119))</f>
         <v/>
@@ -6900,7 +6810,7 @@
         <v/>
       </c>
       <c r="U119" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V119" s="0" t="n">
@@ -6916,7 +6826,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J120" s="9" t="str">
         <f aca="true">IF(M120="", IF(O120="","",X120+(INDIRECT("S" &amp; ROW() - 1) - S120)),IF(O120="", "", INDIRECT("S" &amp; ROW() - 1) - S120))</f>
         <v/>
@@ -6951,7 +6861,7 @@
         <v/>
       </c>
       <c r="U120" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V120" s="0" t="n">
@@ -6967,7 +6877,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J121" s="9" t="str">
         <f aca="true">IF(M121="", IF(O121="","",X121+(INDIRECT("S" &amp; ROW() - 1) - S121)),IF(O121="", "", INDIRECT("S" &amp; ROW() - 1) - S121))</f>
         <v/>
@@ -7002,7 +6912,7 @@
         <v/>
       </c>
       <c r="U121" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V121" s="0" t="n">
@@ -7018,7 +6928,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J122" s="9" t="str">
         <f aca="true">IF(M122="", IF(O122="","",X122+(INDIRECT("S" &amp; ROW() - 1) - S122)),IF(O122="", "", INDIRECT("S" &amp; ROW() - 1) - S122))</f>
         <v/>
@@ -7053,7 +6963,7 @@
         <v/>
       </c>
       <c r="U122" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V122" s="0" t="n">
@@ -7686,26 +7596,26 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="B2:B122" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="B2:B122" type="list">
       <formula1>'Типы варок'!$A$1:$A$102</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="E2:F122" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="E2:F122" type="list">
       <formula1>'Форм фактор плавления'!$A$1:$A$25</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="L1:L122" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="L1:L122" type="list">
       <formula1>Мойки!$A$1:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="H2:H200" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="H2:H200" type="list">
       <formula1>'Вода SKU'!$A$1:$A$150</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7714,21 +7624,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:X287"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.36"/>
@@ -7748,8 +7657,7 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="21" min="21" style="0" width="6.64"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="22" style="0" width="14.54"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="23" min="23" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="24" min="24" style="0" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="25" min="24" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7823,7 +7731,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J2" s="9" t="str">
         <f aca="true">IF(M2="", IF(O2="","",X2+(INDIRECT("S" &amp; ROW() - 1) - S2)),IF(O2="", "", INDIRECT("S" &amp; ROW() - 1) - S2))</f>
         <v/>
@@ -7858,7 +7766,7 @@
         <v/>
       </c>
       <c r="U2" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V2" s="0" t="n">
@@ -7874,7 +7782,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J3" s="9" t="str">
         <f aca="true">IF(M3="", IF(O3="","",X3+(INDIRECT("S" &amp; ROW() - 1) - S3)),IF(O3="", "", INDIRECT("S" &amp; ROW() - 1) - S3))</f>
         <v/>
@@ -7909,7 +7817,7 @@
         <v/>
       </c>
       <c r="U3" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V3" s="0" t="n">
@@ -7925,7 +7833,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J4" s="9" t="str">
         <f aca="true">IF(M4="", IF(O4="","",X4+(INDIRECT("S" &amp; ROW() - 1) - S4)),IF(O4="", "", INDIRECT("S" &amp; ROW() - 1) - S4))</f>
         <v/>
@@ -7960,7 +7868,7 @@
         <v/>
       </c>
       <c r="U4" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V4" s="0" t="n">
@@ -7976,7 +7884,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J5" s="9" t="str">
         <f aca="true">IF(M5="", IF(O5="","",X5+(INDIRECT("S" &amp; ROW() - 1) - S5)),IF(O5="", "", INDIRECT("S" &amp; ROW() - 1) - S5))</f>
         <v/>
@@ -8011,7 +7919,7 @@
         <v/>
       </c>
       <c r="U5" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V5" s="0" t="n">
@@ -8027,7 +7935,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J6" s="9" t="str">
         <f aca="true">IF(M6="", IF(O6="","",X6+(INDIRECT("S" &amp; ROW() - 1) - S6)),IF(O6="", "", INDIRECT("S" &amp; ROW() - 1) - S6))</f>
         <v/>
@@ -8062,7 +7970,7 @@
         <v/>
       </c>
       <c r="U6" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V6" s="0" t="n">
@@ -8078,7 +7986,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J7" s="9" t="str">
         <f aca="true">IF(M7="", IF(O7="","",X7+(INDIRECT("S" &amp; ROW() - 1) - S7)),IF(O7="", "", INDIRECT("S" &amp; ROW() - 1) - S7))</f>
         <v/>
@@ -8113,7 +8021,7 @@
         <v/>
       </c>
       <c r="U7" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V7" s="0" t="n">
@@ -8129,7 +8037,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J8" s="9" t="str">
         <f aca="true">IF(M8="", IF(O8="","",X8+(INDIRECT("S" &amp; ROW() - 1) - S8)),IF(O8="", "", INDIRECT("S" &amp; ROW() - 1) - S8))</f>
         <v/>
@@ -8164,7 +8072,7 @@
         <v/>
       </c>
       <c r="U8" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V8" s="0" t="n">
@@ -8180,7 +8088,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J9" s="9" t="str">
         <f aca="true">IF(M9="", IF(O9="","",X9+(INDIRECT("S" &amp; ROW() - 1) - S9)),IF(O9="", "", INDIRECT("S" &amp; ROW() - 1) - S9))</f>
         <v/>
@@ -8215,7 +8123,7 @@
         <v/>
       </c>
       <c r="U9" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V9" s="0" t="n">
@@ -8231,7 +8139,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J10" s="9" t="str">
         <f aca="true">IF(M10="", IF(O10="","",X10+(INDIRECT("S" &amp; ROW() - 1) - S10)),IF(O10="", "", INDIRECT("S" &amp; ROW() - 1) - S10))</f>
         <v/>
@@ -8266,7 +8174,7 @@
         <v/>
       </c>
       <c r="U10" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V10" s="0" t="n">
@@ -8282,7 +8190,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J11" s="9" t="str">
         <f aca="true">IF(M11="", IF(O11="","",X11+(INDIRECT("S" &amp; ROW() - 1) - S11)),IF(O11="", "", INDIRECT("S" &amp; ROW() - 1) - S11))</f>
         <v/>
@@ -8317,7 +8225,7 @@
         <v/>
       </c>
       <c r="U11" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V11" s="0" t="n">
@@ -8333,7 +8241,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J12" s="9" t="str">
         <f aca="true">IF(M12="", IF(O12="","",X12+(INDIRECT("S" &amp; ROW() - 1) - S12)),IF(O12="", "", INDIRECT("S" &amp; ROW() - 1) - S12))</f>
         <v/>
@@ -8368,7 +8276,7 @@
         <v/>
       </c>
       <c r="U12" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V12" s="0" t="n">
@@ -8384,7 +8292,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J13" s="9" t="str">
         <f aca="true">IF(M13="", IF(O13="","",X13+(INDIRECT("S" &amp; ROW() - 1) - S13)),IF(O13="", "", INDIRECT("S" &amp; ROW() - 1) - S13))</f>
         <v/>
@@ -8419,7 +8327,7 @@
         <v/>
       </c>
       <c r="U13" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V13" s="0" t="n">
@@ -8435,7 +8343,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J14" s="9" t="str">
         <f aca="true">IF(M14="", IF(O14="","",X14+(INDIRECT("S" &amp; ROW() - 1) - S14)),IF(O14="", "", INDIRECT("S" &amp; ROW() - 1) - S14))</f>
         <v/>
@@ -8470,7 +8378,7 @@
         <v/>
       </c>
       <c r="U14" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V14" s="0" t="n">
@@ -8486,7 +8394,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J15" s="9" t="str">
         <f aca="true">IF(M15="", IF(O15="","",X15+(INDIRECT("S" &amp; ROW() - 1) - S15)),IF(O15="", "", INDIRECT("S" &amp; ROW() - 1) - S15))</f>
         <v/>
@@ -8521,7 +8429,7 @@
         <v/>
       </c>
       <c r="U15" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V15" s="0" t="n">
@@ -8537,7 +8445,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J16" s="9" t="str">
         <f aca="true">IF(M16="", IF(O16="","",X16+(INDIRECT("S" &amp; ROW() - 1) - S16)),IF(O16="", "", INDIRECT("S" &amp; ROW() - 1) - S16))</f>
         <v/>
@@ -8572,7 +8480,7 @@
         <v/>
       </c>
       <c r="U16" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V16" s="0" t="n">
@@ -8588,7 +8496,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J17" s="9" t="str">
         <f aca="true">IF(M17="", IF(O17="","",X17+(INDIRECT("S" &amp; ROW() - 1) - S17)),IF(O17="", "", INDIRECT("S" &amp; ROW() - 1) - S17))</f>
         <v/>
@@ -8623,7 +8531,7 @@
         <v/>
       </c>
       <c r="U17" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V17" s="0" t="n">
@@ -8639,7 +8547,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J18" s="9" t="str">
         <f aca="true">IF(M18="", IF(O18="","",X18+(INDIRECT("S" &amp; ROW() - 1) - S18)),IF(O18="", "", INDIRECT("S" &amp; ROW() - 1) - S18))</f>
         <v/>
@@ -8674,7 +8582,7 @@
         <v/>
       </c>
       <c r="U18" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V18" s="0" t="n">
@@ -8690,7 +8598,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J19" s="9" t="str">
         <f aca="true">IF(M19="", IF(O19="","",X19+(INDIRECT("S" &amp; ROW() - 1) - S19)),IF(O19="", "", INDIRECT("S" &amp; ROW() - 1) - S19))</f>
         <v/>
@@ -8725,7 +8633,7 @@
         <v/>
       </c>
       <c r="U19" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V19" s="0" t="n">
@@ -8741,7 +8649,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J20" s="9" t="str">
         <f aca="true">IF(M20="", IF(O20="","",X20+(INDIRECT("S" &amp; ROW() - 1) - S20)),IF(O20="", "", INDIRECT("S" &amp; ROW() - 1) - S20))</f>
         <v/>
@@ -8776,7 +8684,7 @@
         <v/>
       </c>
       <c r="U20" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V20" s="0" t="n">
@@ -8792,7 +8700,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J21" s="9" t="str">
         <f aca="true">IF(M21="", IF(O21="","",X21+(INDIRECT("S" &amp; ROW() - 1) - S21)),IF(O21="", "", INDIRECT("S" &amp; ROW() - 1) - S21))</f>
         <v/>
@@ -8827,7 +8735,7 @@
         <v/>
       </c>
       <c r="U21" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V21" s="0" t="n">
@@ -8843,7 +8751,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J22" s="9" t="str">
         <f aca="true">IF(M22="", IF(O22="","",X22+(INDIRECT("S" &amp; ROW() - 1) - S22)),IF(O22="", "", INDIRECT("S" &amp; ROW() - 1) - S22))</f>
         <v/>
@@ -8878,7 +8786,7 @@
         <v/>
       </c>
       <c r="U22" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V22" s="0" t="n">
@@ -8894,7 +8802,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J23" s="9" t="str">
         <f aca="true">IF(M23="", IF(O23="","",X23+(INDIRECT("S" &amp; ROW() - 1) - S23)),IF(O23="", "", INDIRECT("S" &amp; ROW() - 1) - S23))</f>
         <v/>
@@ -8929,7 +8837,7 @@
         <v/>
       </c>
       <c r="U23" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V23" s="0" t="n">
@@ -8945,7 +8853,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J24" s="9" t="str">
         <f aca="true">IF(M24="", IF(O24="","",X24+(INDIRECT("S" &amp; ROW() - 1) - S24)),IF(O24="", "", INDIRECT("S" &amp; ROW() - 1) - S24))</f>
         <v/>
@@ -8980,7 +8888,7 @@
         <v/>
       </c>
       <c r="U24" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V24" s="0" t="n">
@@ -8996,7 +8904,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J25" s="9" t="str">
         <f aca="true">IF(M25="", IF(O25="","",X25+(INDIRECT("S" &amp; ROW() - 1) - S25)),IF(O25="", "", INDIRECT("S" &amp; ROW() - 1) - S25))</f>
         <v/>
@@ -9031,7 +8939,7 @@
         <v/>
       </c>
       <c r="U25" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V25" s="0" t="n">
@@ -9047,7 +8955,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J26" s="9" t="str">
         <f aca="true">IF(M26="", IF(O26="","",X26+(INDIRECT("S" &amp; ROW() - 1) - S26)),IF(O26="", "", INDIRECT("S" &amp; ROW() - 1) - S26))</f>
         <v/>
@@ -9082,7 +8990,7 @@
         <v/>
       </c>
       <c r="U26" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V26" s="0" t="n">
@@ -9098,7 +9006,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J27" s="9" t="str">
         <f aca="true">IF(M27="", IF(O27="","",X27+(INDIRECT("S" &amp; ROW() - 1) - S27)),IF(O27="", "", INDIRECT("S" &amp; ROW() - 1) - S27))</f>
         <v/>
@@ -9133,7 +9041,7 @@
         <v/>
       </c>
       <c r="U27" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V27" s="0" t="n">
@@ -9149,7 +9057,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J28" s="9" t="str">
         <f aca="true">IF(M28="", IF(O28="","",X28+(INDIRECT("S" &amp; ROW() - 1) - S28)),IF(O28="", "", INDIRECT("S" &amp; ROW() - 1) - S28))</f>
         <v/>
@@ -9184,7 +9092,7 @@
         <v/>
       </c>
       <c r="U28" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V28" s="0" t="n">
@@ -9200,7 +9108,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J29" s="9" t="str">
         <f aca="true">IF(M29="", IF(O29="","",X29+(INDIRECT("S" &amp; ROW() - 1) - S29)),IF(O29="", "", INDIRECT("S" &amp; ROW() - 1) - S29))</f>
         <v/>
@@ -9235,7 +9143,7 @@
         <v/>
       </c>
       <c r="U29" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V29" s="0" t="n">
@@ -9251,7 +9159,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J30" s="9" t="str">
         <f aca="true">IF(M30="", IF(O30="","",X30+(INDIRECT("S" &amp; ROW() - 1) - S30)),IF(O30="", "", INDIRECT("S" &amp; ROW() - 1) - S30))</f>
         <v/>
@@ -9286,7 +9194,7 @@
         <v/>
       </c>
       <c r="U30" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V30" s="0" t="n">
@@ -9302,7 +9210,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J31" s="9" t="str">
         <f aca="true">IF(M31="", IF(O31="","",X31+(INDIRECT("S" &amp; ROW() - 1) - S31)),IF(O31="", "", INDIRECT("S" &amp; ROW() - 1) - S31))</f>
         <v/>
@@ -9337,7 +9245,7 @@
         <v/>
       </c>
       <c r="U31" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V31" s="0" t="n">
@@ -9353,7 +9261,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J32" s="9" t="str">
         <f aca="true">IF(M32="", IF(O32="","",X32+(INDIRECT("S" &amp; ROW() - 1) - S32)),IF(O32="", "", INDIRECT("S" &amp; ROW() - 1) - S32))</f>
         <v/>
@@ -9388,7 +9296,7 @@
         <v/>
       </c>
       <c r="U32" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V32" s="0" t="n">
@@ -9404,7 +9312,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J33" s="9" t="str">
         <f aca="true">IF(M33="", IF(O33="","",X33+(INDIRECT("S" &amp; ROW() - 1) - S33)),IF(O33="", "", INDIRECT("S" &amp; ROW() - 1) - S33))</f>
         <v/>
@@ -9439,7 +9347,7 @@
         <v/>
       </c>
       <c r="U33" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V33" s="0" t="n">
@@ -9455,7 +9363,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J34" s="9" t="str">
         <f aca="true">IF(M34="", IF(O34="","",X34+(INDIRECT("S" &amp; ROW() - 1) - S34)),IF(O34="", "", INDIRECT("S" &amp; ROW() - 1) - S34))</f>
         <v/>
@@ -9490,7 +9398,7 @@
         <v/>
       </c>
       <c r="U34" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V34" s="0" t="n">
@@ -9506,7 +9414,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J35" s="9" t="str">
         <f aca="true">IF(M35="", IF(O35="","",X35+(INDIRECT("S" &amp; ROW() - 1) - S35)),IF(O35="", "", INDIRECT("S" &amp; ROW() - 1) - S35))</f>
         <v/>
@@ -9541,7 +9449,7 @@
         <v/>
       </c>
       <c r="U35" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V35" s="0" t="n">
@@ -9557,7 +9465,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J36" s="9" t="str">
         <f aca="true">IF(M36="", IF(O36="","",X36+(INDIRECT("S" &amp; ROW() - 1) - S36)),IF(O36="", "", INDIRECT("S" &amp; ROW() - 1) - S36))</f>
         <v/>
@@ -9592,7 +9500,7 @@
         <v/>
       </c>
       <c r="U36" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V36" s="0" t="n">
@@ -9608,7 +9516,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J37" s="9" t="str">
         <f aca="true">IF(M37="", IF(O37="","",X37+(INDIRECT("S" &amp; ROW() - 1) - S37)),IF(O37="", "", INDIRECT("S" &amp; ROW() - 1) - S37))</f>
         <v/>
@@ -9643,7 +9551,7 @@
         <v/>
       </c>
       <c r="U37" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V37" s="0" t="n">
@@ -9659,7 +9567,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J38" s="9" t="str">
         <f aca="true">IF(M38="", IF(O38="","",X38+(INDIRECT("S" &amp; ROW() - 1) - S38)),IF(O38="", "", INDIRECT("S" &amp; ROW() - 1) - S38))</f>
         <v/>
@@ -9694,7 +9602,7 @@
         <v/>
       </c>
       <c r="U38" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V38" s="0" t="n">
@@ -9710,7 +9618,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J39" s="9" t="str">
         <f aca="true">IF(M39="", IF(O39="","",X39+(INDIRECT("S" &amp; ROW() - 1) - S39)),IF(O39="", "", INDIRECT("S" &amp; ROW() - 1) - S39))</f>
         <v/>
@@ -9745,7 +9653,7 @@
         <v/>
       </c>
       <c r="U39" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V39" s="0" t="n">
@@ -9761,7 +9669,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J40" s="9" t="str">
         <f aca="true">IF(M40="", IF(O40="","",X40+(INDIRECT("S" &amp; ROW() - 1) - S40)),IF(O40="", "", INDIRECT("S" &amp; ROW() - 1) - S40))</f>
         <v/>
@@ -9796,7 +9704,7 @@
         <v/>
       </c>
       <c r="U40" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V40" s="0" t="n">
@@ -9812,7 +9720,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J41" s="9" t="str">
         <f aca="true">IF(M41="", IF(O41="","",X41+(INDIRECT("S" &amp; ROW() - 1) - S41)),IF(O41="", "", INDIRECT("S" &amp; ROW() - 1) - S41))</f>
         <v/>
@@ -9847,7 +9755,7 @@
         <v/>
       </c>
       <c r="U41" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V41" s="0" t="n">
@@ -9863,7 +9771,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J42" s="9" t="str">
         <f aca="true">IF(M42="", IF(O42="","",X42+(INDIRECT("S" &amp; ROW() - 1) - S42)),IF(O42="", "", INDIRECT("S" &amp; ROW() - 1) - S42))</f>
         <v/>
@@ -9898,7 +9806,7 @@
         <v/>
       </c>
       <c r="U42" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V42" s="0" t="n">
@@ -9914,7 +9822,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J43" s="9" t="str">
         <f aca="true">IF(M43="", IF(O43="","",X43+(INDIRECT("S" &amp; ROW() - 1) - S43)),IF(O43="", "", INDIRECT("S" &amp; ROW() - 1) - S43))</f>
         <v/>
@@ -9949,7 +9857,7 @@
         <v/>
       </c>
       <c r="U43" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V43" s="0" t="n">
@@ -9965,7 +9873,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J44" s="9" t="str">
         <f aca="true">IF(M44="", IF(O44="","",X44+(INDIRECT("S" &amp; ROW() - 1) - S44)),IF(O44="", "", INDIRECT("S" &amp; ROW() - 1) - S44))</f>
         <v/>
@@ -10000,7 +9908,7 @@
         <v/>
       </c>
       <c r="U44" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V44" s="0" t="n">
@@ -10016,7 +9924,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J45" s="9" t="str">
         <f aca="true">IF(M45="", IF(O45="","",X45+(INDIRECT("S" &amp; ROW() - 1) - S45)),IF(O45="", "", INDIRECT("S" &amp; ROW() - 1) - S45))</f>
         <v/>
@@ -10051,7 +9959,7 @@
         <v/>
       </c>
       <c r="U45" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V45" s="0" t="n">
@@ -10067,7 +9975,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J46" s="9" t="str">
         <f aca="true">IF(M46="", IF(O46="","",X46+(INDIRECT("S" &amp; ROW() - 1) - S46)),IF(O46="", "", INDIRECT("S" &amp; ROW() - 1) - S46))</f>
         <v/>
@@ -10102,7 +10010,7 @@
         <v/>
       </c>
       <c r="U46" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V46" s="0" t="n">
@@ -10118,7 +10026,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J47" s="9" t="str">
         <f aca="true">IF(M47="", IF(O47="","",X47+(INDIRECT("S" &amp; ROW() - 1) - S47)),IF(O47="", "", INDIRECT("S" &amp; ROW() - 1) - S47))</f>
         <v/>
@@ -10153,7 +10061,7 @@
         <v/>
       </c>
       <c r="U47" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V47" s="0" t="n">
@@ -10169,7 +10077,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J48" s="9" t="str">
         <f aca="true">IF(M48="", IF(O48="","",X48+(INDIRECT("S" &amp; ROW() - 1) - S48)),IF(O48="", "", INDIRECT("S" &amp; ROW() - 1) - S48))</f>
         <v/>
@@ -10204,7 +10112,7 @@
         <v/>
       </c>
       <c r="U48" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V48" s="0" t="n">
@@ -10220,7 +10128,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J49" s="9" t="str">
         <f aca="true">IF(M49="", IF(O49="","",X49+(INDIRECT("S" &amp; ROW() - 1) - S49)),IF(O49="", "", INDIRECT("S" &amp; ROW() - 1) - S49))</f>
         <v/>
@@ -10255,7 +10163,7 @@
         <v/>
       </c>
       <c r="U49" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V49" s="0" t="n">
@@ -10271,7 +10179,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J50" s="9" t="str">
         <f aca="true">IF(M50="", IF(O50="","",X50+(INDIRECT("S" &amp; ROW() - 1) - S50)),IF(O50="", "", INDIRECT("S" &amp; ROW() - 1) - S50))</f>
         <v/>
@@ -10306,7 +10214,7 @@
         <v/>
       </c>
       <c r="U50" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V50" s="0" t="n">
@@ -10322,7 +10230,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J51" s="9" t="str">
         <f aca="true">IF(M51="", IF(O51="","",X51+(INDIRECT("S" &amp; ROW() - 1) - S51)),IF(O51="", "", INDIRECT("S" &amp; ROW() - 1) - S51))</f>
         <v/>
@@ -10357,7 +10265,7 @@
         <v/>
       </c>
       <c r="U51" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V51" s="0" t="n">
@@ -10373,7 +10281,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J52" s="9" t="str">
         <f aca="true">IF(M52="", IF(O52="","",X52+(INDIRECT("S" &amp; ROW() - 1) - S52)),IF(O52="", "", INDIRECT("S" &amp; ROW() - 1) - S52))</f>
         <v/>
@@ -10408,7 +10316,7 @@
         <v/>
       </c>
       <c r="U52" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V52" s="0" t="n">
@@ -10424,7 +10332,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J53" s="9" t="str">
         <f aca="true">IF(M53="", IF(O53="","",X53+(INDIRECT("S" &amp; ROW() - 1) - S53)),IF(O53="", "", INDIRECT("S" &amp; ROW() - 1) - S53))</f>
         <v/>
@@ -10459,7 +10367,7 @@
         <v/>
       </c>
       <c r="U53" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V53" s="0" t="n">
@@ -10475,7 +10383,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J54" s="9" t="str">
         <f aca="true">IF(M54="", IF(O54="","",X54+(INDIRECT("S" &amp; ROW() - 1) - S54)),IF(O54="", "", INDIRECT("S" &amp; ROW() - 1) - S54))</f>
         <v/>
@@ -10510,7 +10418,7 @@
         <v/>
       </c>
       <c r="U54" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V54" s="0" t="n">
@@ -10526,7 +10434,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J55" s="9" t="str">
         <f aca="true">IF(M55="", IF(O55="","",X55+(INDIRECT("S" &amp; ROW() - 1) - S55)),IF(O55="", "", INDIRECT("S" &amp; ROW() - 1) - S55))</f>
         <v/>
@@ -10561,7 +10469,7 @@
         <v/>
       </c>
       <c r="U55" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V55" s="0" t="n">
@@ -10577,7 +10485,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J56" s="9" t="str">
         <f aca="true">IF(M56="", IF(O56="","",X56+(INDIRECT("S" &amp; ROW() - 1) - S56)),IF(O56="", "", INDIRECT("S" &amp; ROW() - 1) - S56))</f>
         <v/>
@@ -10612,7 +10520,7 @@
         <v/>
       </c>
       <c r="U56" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V56" s="0" t="n">
@@ -10628,7 +10536,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J57" s="9" t="str">
         <f aca="true">IF(M57="", IF(O57="","",X57+(INDIRECT("S" &amp; ROW() - 1) - S57)),IF(O57="", "", INDIRECT("S" &amp; ROW() - 1) - S57))</f>
         <v/>
@@ -10663,7 +10571,7 @@
         <v/>
       </c>
       <c r="U57" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V57" s="0" t="n">
@@ -10679,7 +10587,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J58" s="9" t="str">
         <f aca="true">IF(M58="", IF(O58="","",X58+(INDIRECT("S" &amp; ROW() - 1) - S58)),IF(O58="", "", INDIRECT("S" &amp; ROW() - 1) - S58))</f>
         <v/>
@@ -10714,7 +10622,7 @@
         <v/>
       </c>
       <c r="U58" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V58" s="0" t="n">
@@ -10730,7 +10638,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J59" s="9" t="str">
         <f aca="true">IF(M59="", IF(O59="","",X59+(INDIRECT("S" &amp; ROW() - 1) - S59)),IF(O59="", "", INDIRECT("S" &amp; ROW() - 1) - S59))</f>
         <v/>
@@ -10765,7 +10673,7 @@
         <v/>
       </c>
       <c r="U59" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V59" s="0" t="n">
@@ -10781,7 +10689,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J60" s="9" t="str">
         <f aca="true">IF(M60="", IF(O60="","",X60+(INDIRECT("S" &amp; ROW() - 1) - S60)),IF(O60="", "", INDIRECT("S" &amp; ROW() - 1) - S60))</f>
         <v/>
@@ -10816,7 +10724,7 @@
         <v/>
       </c>
       <c r="U60" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V60" s="0" t="n">
@@ -10832,7 +10740,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J61" s="9" t="str">
         <f aca="true">IF(M61="", IF(O61="","",X61+(INDIRECT("S" &amp; ROW() - 1) - S61)),IF(O61="", "", INDIRECT("S" &amp; ROW() - 1) - S61))</f>
         <v/>
@@ -10867,7 +10775,7 @@
         <v/>
       </c>
       <c r="U61" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V61" s="0" t="n">
@@ -10883,7 +10791,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J62" s="9" t="str">
         <f aca="true">IF(M62="", IF(O62="","",X62+(INDIRECT("S" &amp; ROW() - 1) - S62)),IF(O62="", "", INDIRECT("S" &amp; ROW() - 1) - S62))</f>
         <v/>
@@ -10918,7 +10826,7 @@
         <v/>
       </c>
       <c r="U62" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V62" s="0" t="n">
@@ -10934,7 +10842,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J63" s="9" t="str">
         <f aca="true">IF(M63="", IF(O63="","",X63+(INDIRECT("S" &amp; ROW() - 1) - S63)),IF(O63="", "", INDIRECT("S" &amp; ROW() - 1) - S63))</f>
         <v/>
@@ -10969,7 +10877,7 @@
         <v/>
       </c>
       <c r="U63" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V63" s="0" t="n">
@@ -10985,7 +10893,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J64" s="9" t="str">
         <f aca="true">IF(M64="", IF(O64="","",X64+(INDIRECT("S" &amp; ROW() - 1) - S64)),IF(O64="", "", INDIRECT("S" &amp; ROW() - 1) - S64))</f>
         <v/>
@@ -11020,7 +10928,7 @@
         <v/>
       </c>
       <c r="U64" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V64" s="0" t="n">
@@ -11036,7 +10944,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J65" s="9" t="str">
         <f aca="true">IF(M65="", IF(O65="","",X65+(INDIRECT("S" &amp; ROW() - 1) - S65)),IF(O65="", "", INDIRECT("S" &amp; ROW() - 1) - S65))</f>
         <v/>
@@ -11071,7 +10979,7 @@
         <v/>
       </c>
       <c r="U65" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V65" s="0" t="n">
@@ -11087,7 +10995,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J66" s="9" t="str">
         <f aca="true">IF(M66="", IF(O66="","",X66+(INDIRECT("S" &amp; ROW() - 1) - S66)),IF(O66="", "", INDIRECT("S" &amp; ROW() - 1) - S66))</f>
         <v/>
@@ -11122,7 +11030,7 @@
         <v/>
       </c>
       <c r="U66" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V66" s="0" t="n">
@@ -11138,7 +11046,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J67" s="9" t="str">
         <f aca="true">IF(M67="", IF(O67="","",X67+(INDIRECT("S" &amp; ROW() - 1) - S67)),IF(O67="", "", INDIRECT("S" &amp; ROW() - 1) - S67))</f>
         <v/>
@@ -11173,7 +11081,7 @@
         <v/>
       </c>
       <c r="U67" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V67" s="0" t="n">
@@ -11189,7 +11097,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J68" s="9" t="str">
         <f aca="true">IF(M68="", IF(O68="","",X68+(INDIRECT("S" &amp; ROW() - 1) - S68)),IF(O68="", "", INDIRECT("S" &amp; ROW() - 1) - S68))</f>
         <v/>
@@ -11224,7 +11132,7 @@
         <v/>
       </c>
       <c r="U68" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V68" s="0" t="n">
@@ -11240,7 +11148,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J69" s="9" t="str">
         <f aca="true">IF(M69="", IF(O69="","",X69+(INDIRECT("S" &amp; ROW() - 1) - S69)),IF(O69="", "", INDIRECT("S" &amp; ROW() - 1) - S69))</f>
         <v/>
@@ -11275,7 +11183,7 @@
         <v/>
       </c>
       <c r="U69" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V69" s="0" t="n">
@@ -11291,7 +11199,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J70" s="9" t="str">
         <f aca="true">IF(M70="", IF(O70="","",X70+(INDIRECT("S" &amp; ROW() - 1) - S70)),IF(O70="", "", INDIRECT("S" &amp; ROW() - 1) - S70))</f>
         <v/>
@@ -11326,7 +11234,7 @@
         <v/>
       </c>
       <c r="U70" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V70" s="0" t="n">
@@ -11342,7 +11250,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J71" s="9" t="str">
         <f aca="true">IF(M71="", IF(O71="","",X71+(INDIRECT("S" &amp; ROW() - 1) - S71)),IF(O71="", "", INDIRECT("S" &amp; ROW() - 1) - S71))</f>
         <v/>
@@ -11377,7 +11285,7 @@
         <v/>
       </c>
       <c r="U71" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V71" s="0" t="n">
@@ -11393,7 +11301,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J72" s="9" t="str">
         <f aca="true">IF(M72="", IF(O72="","",X72+(INDIRECT("S" &amp; ROW() - 1) - S72)),IF(O72="", "", INDIRECT("S" &amp; ROW() - 1) - S72))</f>
         <v/>
@@ -11428,7 +11336,7 @@
         <v/>
       </c>
       <c r="U72" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V72" s="0" t="n">
@@ -11444,7 +11352,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J73" s="9" t="str">
         <f aca="true">IF(M73="", IF(O73="","",X73+(INDIRECT("S" &amp; ROW() - 1) - S73)),IF(O73="", "", INDIRECT("S" &amp; ROW() - 1) - S73))</f>
         <v/>
@@ -11479,7 +11387,7 @@
         <v/>
       </c>
       <c r="U73" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V73" s="0" t="n">
@@ -11495,7 +11403,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J74" s="9" t="str">
         <f aca="true">IF(M74="", IF(O74="","",X74+(INDIRECT("S" &amp; ROW() - 1) - S74)),IF(O74="", "", INDIRECT("S" &amp; ROW() - 1) - S74))</f>
         <v/>
@@ -11530,7 +11438,7 @@
         <v/>
       </c>
       <c r="U74" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V74" s="0" t="n">
@@ -11546,7 +11454,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J75" s="9" t="str">
         <f aca="true">IF(M75="", IF(O75="","",X75+(INDIRECT("S" &amp; ROW() - 1) - S75)),IF(O75="", "", INDIRECT("S" &amp; ROW() - 1) - S75))</f>
         <v/>
@@ -11581,7 +11489,7 @@
         <v/>
       </c>
       <c r="U75" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V75" s="0" t="n">
@@ -11597,7 +11505,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J76" s="9" t="str">
         <f aca="true">IF(M76="", IF(O76="","",X76+(INDIRECT("S" &amp; ROW() - 1) - S76)),IF(O76="", "", INDIRECT("S" &amp; ROW() - 1) - S76))</f>
         <v/>
@@ -11632,7 +11540,7 @@
         <v/>
       </c>
       <c r="U76" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V76" s="0" t="n">
@@ -11648,7 +11556,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J77" s="9" t="str">
         <f aca="true">IF(M77="", IF(O77="","",X77+(INDIRECT("S" &amp; ROW() - 1) - S77)),IF(O77="", "", INDIRECT("S" &amp; ROW() - 1) - S77))</f>
         <v/>
@@ -11683,7 +11591,7 @@
         <v/>
       </c>
       <c r="U77" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V77" s="0" t="n">
@@ -11699,7 +11607,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J78" s="9" t="str">
         <f aca="true">IF(M78="", IF(O78="","",X78+(INDIRECT("S" &amp; ROW() - 1) - S78)),IF(O78="", "", INDIRECT("S" &amp; ROW() - 1) - S78))</f>
         <v/>
@@ -11734,7 +11642,7 @@
         <v/>
       </c>
       <c r="U78" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V78" s="0" t="n">
@@ -11750,7 +11658,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J79" s="9" t="str">
         <f aca="true">IF(M79="", IF(O79="","",X79+(INDIRECT("S" &amp; ROW() - 1) - S79)),IF(O79="", "", INDIRECT("S" &amp; ROW() - 1) - S79))</f>
         <v/>
@@ -11785,7 +11693,7 @@
         <v/>
       </c>
       <c r="U79" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V79" s="0" t="n">
@@ -11801,7 +11709,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J80" s="9" t="str">
         <f aca="true">IF(M80="", IF(O80="","",X80+(INDIRECT("S" &amp; ROW() - 1) - S80)),IF(O80="", "", INDIRECT("S" &amp; ROW() - 1) - S80))</f>
         <v/>
@@ -11836,7 +11744,7 @@
         <v/>
       </c>
       <c r="U80" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V80" s="0" t="n">
@@ -11852,7 +11760,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J81" s="9" t="str">
         <f aca="true">IF(M81="", IF(O81="","",X81+(INDIRECT("S" &amp; ROW() - 1) - S81)),IF(O81="", "", INDIRECT("S" &amp; ROW() - 1) - S81))</f>
         <v/>
@@ -11887,7 +11795,7 @@
         <v/>
       </c>
       <c r="U81" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V81" s="0" t="n">
@@ -11903,7 +11811,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J82" s="9" t="str">
         <f aca="true">IF(M82="", IF(O82="","",X82+(INDIRECT("S" &amp; ROW() - 1) - S82)),IF(O82="", "", INDIRECT("S" &amp; ROW() - 1) - S82))</f>
         <v/>
@@ -11938,7 +11846,7 @@
         <v/>
       </c>
       <c r="U82" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V82" s="0" t="n">
@@ -11954,7 +11862,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J83" s="9" t="str">
         <f aca="true">IF(M83="", IF(O83="","",X83+(INDIRECT("S" &amp; ROW() - 1) - S83)),IF(O83="", "", INDIRECT("S" &amp; ROW() - 1) - S83))</f>
         <v/>
@@ -11989,7 +11897,7 @@
         <v/>
       </c>
       <c r="U83" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V83" s="0" t="n">
@@ -12005,7 +11913,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J84" s="9" t="str">
         <f aca="true">IF(M84="", IF(O84="","",X84+(INDIRECT("S" &amp; ROW() - 1) - S84)),IF(O84="", "", INDIRECT("S" &amp; ROW() - 1) - S84))</f>
         <v/>
@@ -12040,7 +11948,7 @@
         <v/>
       </c>
       <c r="U84" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V84" s="0" t="n">
@@ -12056,7 +11964,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J85" s="9" t="str">
         <f aca="true">IF(M85="", IF(O85="","",X85+(INDIRECT("S" &amp; ROW() - 1) - S85)),IF(O85="", "", INDIRECT("S" &amp; ROW() - 1) - S85))</f>
         <v/>
@@ -12091,7 +11999,7 @@
         <v/>
       </c>
       <c r="U85" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V85" s="0" t="n">
@@ -12107,7 +12015,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J86" s="9" t="str">
         <f aca="true">IF(M86="", IF(O86="","",X86+(INDIRECT("S" &amp; ROW() - 1) - S86)),IF(O86="", "", INDIRECT("S" &amp; ROW() - 1) - S86))</f>
         <v/>
@@ -12142,7 +12050,7 @@
         <v/>
       </c>
       <c r="U86" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V86" s="0" t="n">
@@ -12158,7 +12066,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J87" s="9" t="str">
         <f aca="true">IF(M87="", IF(O87="","",X87+(INDIRECT("S" &amp; ROW() - 1) - S87)),IF(O87="", "", INDIRECT("S" &amp; ROW() - 1) - S87))</f>
         <v/>
@@ -12193,7 +12101,7 @@
         <v/>
       </c>
       <c r="U87" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V87" s="0" t="n">
@@ -12209,7 +12117,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J88" s="9" t="str">
         <f aca="true">IF(M88="", IF(O88="","",X88+(INDIRECT("S" &amp; ROW() - 1) - S88)),IF(O88="", "", INDIRECT("S" &amp; ROW() - 1) - S88))</f>
         <v/>
@@ -12244,7 +12152,7 @@
         <v/>
       </c>
       <c r="U88" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V88" s="0" t="n">
@@ -12260,7 +12168,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J89" s="9" t="str">
         <f aca="true">IF(M89="", IF(O89="","",X89+(INDIRECT("S" &amp; ROW() - 1) - S89)),IF(O89="", "", INDIRECT("S" &amp; ROW() - 1) - S89))</f>
         <v/>
@@ -12295,7 +12203,7 @@
         <v/>
       </c>
       <c r="U89" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V89" s="0" t="n">
@@ -12311,7 +12219,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J90" s="9" t="str">
         <f aca="true">IF(M90="", IF(O90="","",X90+(INDIRECT("S" &amp; ROW() - 1) - S90)),IF(O90="", "", INDIRECT("S" &amp; ROW() - 1) - S90))</f>
         <v/>
@@ -12346,7 +12254,7 @@
         <v/>
       </c>
       <c r="U90" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V90" s="0" t="n">
@@ -12362,7 +12270,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J91" s="9" t="str">
         <f aca="true">IF(M91="", IF(O91="","",X91+(INDIRECT("S" &amp; ROW() - 1) - S91)),IF(O91="", "", INDIRECT("S" &amp; ROW() - 1) - S91))</f>
         <v/>
@@ -12397,7 +12305,7 @@
         <v/>
       </c>
       <c r="U91" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V91" s="0" t="n">
@@ -12413,7 +12321,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J92" s="9" t="str">
         <f aca="true">IF(M92="", IF(O92="","",X92+(INDIRECT("S" &amp; ROW() - 1) - S92)),IF(O92="", "", INDIRECT("S" &amp; ROW() - 1) - S92))</f>
         <v/>
@@ -12448,7 +12356,7 @@
         <v/>
       </c>
       <c r="U92" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V92" s="0" t="n">
@@ -12464,7 +12372,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J93" s="9" t="str">
         <f aca="true">IF(M93="", IF(O93="","",X93+(INDIRECT("S" &amp; ROW() - 1) - S93)),IF(O93="", "", INDIRECT("S" &amp; ROW() - 1) - S93))</f>
         <v/>
@@ -12499,7 +12407,7 @@
         <v/>
       </c>
       <c r="U93" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V93" s="0" t="n">
@@ -12515,7 +12423,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J94" s="9" t="str">
         <f aca="true">IF(M94="", IF(O94="","",X94+(INDIRECT("S" &amp; ROW() - 1) - S94)),IF(O94="", "", INDIRECT("S" &amp; ROW() - 1) - S94))</f>
         <v/>
@@ -12550,7 +12458,7 @@
         <v/>
       </c>
       <c r="U94" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V94" s="0" t="n">
@@ -12566,7 +12474,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J95" s="9" t="str">
         <f aca="true">IF(M95="", IF(O95="","",X95+(INDIRECT("S" &amp; ROW() - 1) - S95)),IF(O95="", "", INDIRECT("S" &amp; ROW() - 1) - S95))</f>
         <v/>
@@ -12601,7 +12509,7 @@
         <v/>
       </c>
       <c r="U95" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V95" s="0" t="n">
@@ -12617,7 +12525,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J96" s="9" t="str">
         <f aca="true">IF(M96="", IF(O96="","",X96+(INDIRECT("S" &amp; ROW() - 1) - S96)),IF(O96="", "", INDIRECT("S" &amp; ROW() - 1) - S96))</f>
         <v/>
@@ -12652,7 +12560,7 @@
         <v/>
       </c>
       <c r="U96" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V96" s="0" t="n">
@@ -12668,7 +12576,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J97" s="9" t="str">
         <f aca="true">IF(M97="", IF(O97="","",X97+(INDIRECT("S" &amp; ROW() - 1) - S97)),IF(O97="", "", INDIRECT("S" &amp; ROW() - 1) - S97))</f>
         <v/>
@@ -12703,7 +12611,7 @@
         <v/>
       </c>
       <c r="U97" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V97" s="0" t="n">
@@ -12719,7 +12627,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J98" s="9" t="str">
         <f aca="true">IF(M98="", IF(O98="","",X98+(INDIRECT("S" &amp; ROW() - 1) - S98)),IF(O98="", "", INDIRECT("S" &amp; ROW() - 1) - S98))</f>
         <v/>
@@ -12754,7 +12662,7 @@
         <v/>
       </c>
       <c r="U98" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V98" s="0" t="n">
@@ -12770,7 +12678,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J99" s="9" t="str">
         <f aca="true">IF(M99="", IF(O99="","",X99+(INDIRECT("S" &amp; ROW() - 1) - S99)),IF(O99="", "", INDIRECT("S" &amp; ROW() - 1) - S99))</f>
         <v/>
@@ -12805,7 +12713,7 @@
         <v/>
       </c>
       <c r="U99" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V99" s="0" t="n">
@@ -12821,7 +12729,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J100" s="9" t="str">
         <f aca="true">IF(M100="", IF(O100="","",X100+(INDIRECT("S" &amp; ROW() - 1) - S100)),IF(O100="", "", INDIRECT("S" &amp; ROW() - 1) - S100))</f>
         <v/>
@@ -12856,7 +12764,7 @@
         <v/>
       </c>
       <c r="U100" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V100" s="0" t="n">
@@ -12872,7 +12780,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J101" s="9" t="str">
         <f aca="true">IF(M101="", IF(O101="","",X101+(INDIRECT("S" &amp; ROW() - 1) - S101)),IF(O101="", "", INDIRECT("S" &amp; ROW() - 1) - S101))</f>
         <v/>
@@ -12907,7 +12815,7 @@
         <v/>
       </c>
       <c r="U101" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V101" s="0" t="n">
@@ -12923,7 +12831,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J102" s="9" t="str">
         <f aca="true">IF(M102="", IF(O102="","",X102+(INDIRECT("S" &amp; ROW() - 1) - S102)),IF(O102="", "", INDIRECT("S" &amp; ROW() - 1) - S102))</f>
         <v/>
@@ -12958,7 +12866,7 @@
         <v/>
       </c>
       <c r="U102" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V102" s="0" t="n">
@@ -12974,7 +12882,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J103" s="9" t="str">
         <f aca="true">IF(M103="", IF(O103="","",X103+(INDIRECT("S" &amp; ROW() - 1) - S103)),IF(O103="", "", INDIRECT("S" &amp; ROW() - 1) - S103))</f>
         <v/>
@@ -13009,7 +12917,7 @@
         <v/>
       </c>
       <c r="U103" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V103" s="0" t="n">
@@ -13025,7 +12933,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J104" s="9" t="str">
         <f aca="true">IF(M104="", IF(O104="","",X104+(INDIRECT("S" &amp; ROW() - 1) - S104)),IF(O104="", "", INDIRECT("S" &amp; ROW() - 1) - S104))</f>
         <v/>
@@ -13060,7 +12968,7 @@
         <v/>
       </c>
       <c r="U104" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V104" s="0" t="n">
@@ -13076,7 +12984,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J105" s="9" t="str">
         <f aca="true">IF(M105="", IF(O105="","",X105+(INDIRECT("S" &amp; ROW() - 1) - S105)),IF(O105="", "", INDIRECT("S" &amp; ROW() - 1) - S105))</f>
         <v/>
@@ -13111,7 +13019,7 @@
         <v/>
       </c>
       <c r="U105" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V105" s="0" t="n">
@@ -13127,7 +13035,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J106" s="9" t="str">
         <f aca="true">IF(M106="", IF(O106="","",X106+(INDIRECT("S" &amp; ROW() - 1) - S106)),IF(O106="", "", INDIRECT("S" &amp; ROW() - 1) - S106))</f>
         <v/>
@@ -13162,7 +13070,7 @@
         <v/>
       </c>
       <c r="U106" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V106" s="0" t="n">
@@ -13178,7 +13086,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J107" s="9" t="str">
         <f aca="true">IF(M107="", IF(O107="","",X107+(INDIRECT("S" &amp; ROW() - 1) - S107)),IF(O107="", "", INDIRECT("S" &amp; ROW() - 1) - S107))</f>
         <v/>
@@ -13213,7 +13121,7 @@
         <v/>
       </c>
       <c r="U107" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V107" s="0" t="n">
@@ -13229,7 +13137,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J108" s="9" t="str">
         <f aca="true">IF(M108="", IF(O108="","",X108+(INDIRECT("S" &amp; ROW() - 1) - S108)),IF(O108="", "", INDIRECT("S" &amp; ROW() - 1) - S108))</f>
         <v/>
@@ -13264,7 +13172,7 @@
         <v/>
       </c>
       <c r="U108" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V108" s="0" t="n">
@@ -13280,7 +13188,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J109" s="9" t="str">
         <f aca="true">IF(M109="", IF(O109="","",X109+(INDIRECT("S" &amp; ROW() - 1) - S109)),IF(O109="", "", INDIRECT("S" &amp; ROW() - 1) - S109))</f>
         <v/>
@@ -13315,7 +13223,7 @@
         <v/>
       </c>
       <c r="U109" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V109" s="0" t="n">
@@ -13331,7 +13239,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J110" s="9" t="str">
         <f aca="true">IF(M110="", IF(O110="","",X110+(INDIRECT("S" &amp; ROW() - 1) - S110)),IF(O110="", "", INDIRECT("S" &amp; ROW() - 1) - S110))</f>
         <v/>
@@ -13366,7 +13274,7 @@
         <v/>
       </c>
       <c r="U110" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V110" s="0" t="n">
@@ -13382,7 +13290,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J111" s="9" t="str">
         <f aca="true">IF(M111="", IF(O111="","",X111+(INDIRECT("S" &amp; ROW() - 1) - S111)),IF(O111="", "", INDIRECT("S" &amp; ROW() - 1) - S111))</f>
         <v/>
@@ -13417,7 +13325,7 @@
         <v/>
       </c>
       <c r="U111" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V111" s="0" t="n">
@@ -13433,7 +13341,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J112" s="9" t="str">
         <f aca="true">IF(M112="", IF(O112="","",X112+(INDIRECT("S" &amp; ROW() - 1) - S112)),IF(O112="", "", INDIRECT("S" &amp; ROW() - 1) - S112))</f>
         <v/>
@@ -13468,7 +13376,7 @@
         <v/>
       </c>
       <c r="U112" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V112" s="0" t="n">
@@ -13484,7 +13392,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J113" s="9" t="str">
         <f aca="true">IF(M113="", IF(O113="","",X113+(INDIRECT("S" &amp; ROW() - 1) - S113)),IF(O113="", "", INDIRECT("S" &amp; ROW() - 1) - S113))</f>
         <v/>
@@ -13519,7 +13427,7 @@
         <v/>
       </c>
       <c r="U113" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V113" s="0" t="n">
@@ -13535,7 +13443,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J114" s="9" t="str">
         <f aca="true">IF(M114="", IF(O114="","",X114+(INDIRECT("S" &amp; ROW() - 1) - S114)),IF(O114="", "", INDIRECT("S" &amp; ROW() - 1) - S114))</f>
         <v/>
@@ -13570,7 +13478,7 @@
         <v/>
       </c>
       <c r="U114" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V114" s="0" t="n">
@@ -13586,7 +13494,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J115" s="9" t="str">
         <f aca="true">IF(M115="", IF(O115="","",X115+(INDIRECT("S" &amp; ROW() - 1) - S115)),IF(O115="", "", INDIRECT("S" &amp; ROW() - 1) - S115))</f>
         <v/>
@@ -13621,7 +13529,7 @@
         <v/>
       </c>
       <c r="U115" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V115" s="0" t="n">
@@ -13637,7 +13545,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J116" s="9" t="str">
         <f aca="true">IF(M116="", IF(O116="","",X116+(INDIRECT("S" &amp; ROW() - 1) - S116)),IF(O116="", "", INDIRECT("S" &amp; ROW() - 1) - S116))</f>
         <v/>
@@ -13672,7 +13580,7 @@
         <v/>
       </c>
       <c r="U116" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V116" s="0" t="n">
@@ -13688,7 +13596,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J117" s="9" t="str">
         <f aca="true">IF(M117="", IF(O117="","",X117+(INDIRECT("S" &amp; ROW() - 1) - S117)),IF(O117="", "", INDIRECT("S" &amp; ROW() - 1) - S117))</f>
         <v/>
@@ -13723,7 +13631,7 @@
         <v/>
       </c>
       <c r="U117" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V117" s="0" t="n">
@@ -13739,7 +13647,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J118" s="9" t="str">
         <f aca="true">IF(M118="", IF(O118="","",X118+(INDIRECT("S" &amp; ROW() - 1) - S118)),IF(O118="", "", INDIRECT("S" &amp; ROW() - 1) - S118))</f>
         <v/>
@@ -13774,7 +13682,7 @@
         <v/>
       </c>
       <c r="U118" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V118" s="0" t="n">
@@ -13790,7 +13698,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J119" s="9" t="str">
         <f aca="true">IF(M119="", IF(O119="","",X119+(INDIRECT("S" &amp; ROW() - 1) - S119)),IF(O119="", "", INDIRECT("S" &amp; ROW() - 1) - S119))</f>
         <v/>
@@ -13825,7 +13733,7 @@
         <v/>
       </c>
       <c r="U119" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V119" s="0" t="n">
@@ -13841,7 +13749,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J120" s="9" t="str">
         <f aca="true">IF(M120="", IF(O120="","",X120+(INDIRECT("S" &amp; ROW() - 1) - S120)),IF(O120="", "", INDIRECT("S" &amp; ROW() - 1) - S120))</f>
         <v/>
@@ -13876,7 +13784,7 @@
         <v/>
       </c>
       <c r="U120" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V120" s="0" t="n">
@@ -13892,7 +13800,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J121" s="9" t="str">
         <f aca="true">IF(M121="", IF(O121="","",X121+(INDIRECT("S" &amp; ROW() - 1) - S121)),IF(O121="", "", INDIRECT("S" &amp; ROW() - 1) - S121))</f>
         <v/>
@@ -13927,7 +13835,7 @@
         <v/>
       </c>
       <c r="U121" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V121" s="0" t="n">
@@ -13943,7 +13851,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J122" s="9" t="str">
         <f aca="true">IF(M122="", IF(O122="","",X122+(INDIRECT("S" &amp; ROW() - 1) - S122)),IF(O122="", "", INDIRECT("S" &amp; ROW() - 1) - S122))</f>
         <v/>
@@ -13978,7 +13886,7 @@
         <v/>
       </c>
       <c r="U122" s="0" t="n">
-        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8000/OFFSET($C$1, 1, 0))</f>
+        <f aca="true">IF(OFFSET($C$1, 1, 0)="", 1, 8300/OFFSET($C$1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="V122" s="0" t="n">
@@ -15010,26 +14918,26 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="B2:B122" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="B2:B122" type="list">
       <formula1>'Типы варок'!$A$1:$A$102</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="E2:F122" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="E2:F122" type="list">
       <formula1>'Форм фактор плавления'!$A$1:$A$25</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="L1:L122" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="L1:L122" type="list">
       <formula1>Мойки!$A$1:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="H2:H200" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="H2:H200" type="list">
       <formula1>'Соль SKU'!$A$1:$A$150</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -15038,7 +14946,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -15048,10 +14956,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.54"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -15070,8 +14975,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -15080,7 +14985,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -15090,15 +14995,14 @@
       <selection pane="topLeft" activeCell="G48" activeCellId="0" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="9.09"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -15107,7 +15011,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -15117,14 +15021,14 @@
       <selection pane="topLeft" activeCell="N10" activeCellId="0" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="23" width="9.09"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="23" width="9.09"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -15133,7 +15037,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -15143,14 +15047,11 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.54"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -15159,7 +15060,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -15169,15 +15070,14 @@
       <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.54"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>